<commit_message>
Actualización de archivos en la carpeta data - 2025-01-30 15:42:14
</commit_message>
<xml_diff>
--- a/data/Informe_Diario_Unidades.xlsx
+++ b/data/Informe_Diario_Unidades.xlsx
@@ -1162,7 +1162,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D30" sqref="D30"/>
+      <selection pane="topRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1305,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Actualización de archivos en la carpeta data - 2025-01-31 12:32:01
</commit_message>
<xml_diff>
--- a/data/Informe_Diario_Unidades.xlsx
+++ b/data/Informe_Diario_Unidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="237">
   <si>
     <t>Operador</t>
   </si>
@@ -114,6 +114,30 @@
     <t>Comer/Beber (Manual)</t>
   </si>
   <si>
+    <t>Eduardo Hernandez</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX</t>
+  </si>
+  <si>
+    <t>03:21:25</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>Jan 30 2:54PM CST</t>
+  </si>
+  <si>
     <t>Christian Aguilar</t>
   </si>
   <si>
@@ -123,34 +147,253 @@
     <t>TOYOTA HILUX 2021</t>
   </si>
   <si>
-    <t>04:00:42</t>
+    <t>02:53:59</t>
+  </si>
+  <si>
+    <t>Jan 30 1:59PM CST</t>
+  </si>
+  <si>
+    <t>Gerardo Aguillón</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>02:25:09</t>
+  </si>
+  <si>
+    <t>Jan 30 12:37PM CST</t>
+  </si>
+  <si>
+    <t>Marcos Barbosa</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2023</t>
+  </si>
+  <si>
+    <t>02:31:56</t>
+  </si>
+  <si>
+    <t>Jan 30 12:56PM CST</t>
+  </si>
+  <si>
+    <t>Hugo López</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>01:39:01</t>
+  </si>
+  <si>
+    <t>00:00:06</t>
+  </si>
+  <si>
+    <t>Jan 30 1:02PM CST</t>
+  </si>
+  <si>
+    <t>Luis Ramirez</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>FORD F350 3MTS 2006</t>
+  </si>
+  <si>
+    <t>01:37:25</t>
+  </si>
+  <si>
+    <t>Jan 30 1:18PM CST</t>
+  </si>
+  <si>
+    <t>Martin Quezada</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>00:14:39</t>
+  </si>
+  <si>
+    <t>Jan 30 5:28PM CST</t>
+  </si>
+  <si>
+    <t>Francisco Marquez</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+  </si>
+  <si>
+    <t>00:01:31</t>
+  </si>
+  <si>
+    <t>Jan 30 7:14PM CST</t>
+  </si>
+  <si>
+    <t>Alejandro Suarez</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>HINO 500</t>
+  </si>
+  <si>
+    <t>00:01:32</t>
+  </si>
+  <si>
+    <t>Jan 30 6:37PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Ornelas</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2020</t>
+  </si>
+  <si>
+    <t>04:00:53</t>
+  </si>
+  <si>
+    <t>00:00:48</t>
+  </si>
+  <si>
+    <t>00:00:36</t>
+  </si>
+  <si>
+    <t>Jan 30 3:20PM CST</t>
+  </si>
+  <si>
+    <t>Diego Cardenas</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2018</t>
+  </si>
+  <si>
+    <t>03:25:16</t>
+  </si>
+  <si>
+    <t>00:01:11</t>
+  </si>
+  <si>
+    <t>00:00:21</t>
+  </si>
+  <si>
+    <t>Jan 30 7:41AM CST</t>
+  </si>
+  <si>
+    <t>José Morales</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>02:21:24</t>
+  </si>
+  <si>
+    <t>00:00:49</t>
+  </si>
+  <si>
+    <t>00:00:33</t>
+  </si>
+  <si>
+    <t>Jan 30 1:11PM CST</t>
+  </si>
+  <si>
+    <t>Kevin De La O</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>VAN HYUNDAI</t>
+  </si>
+  <si>
+    <t>00:37:18</t>
+  </si>
+  <si>
+    <t>00:00:17</t>
+  </si>
+  <si>
+    <t>00:00:09</t>
+  </si>
+  <si>
+    <t>Jan 30 3:35AM CST</t>
+  </si>
+  <si>
+    <t>Eduardo Lopez</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>01:26:14</t>
   </si>
   <si>
     <t>00:00:32</t>
   </si>
   <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
-    <t>Jan 29 11:19AM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Hernandez</t>
-  </si>
-  <si>
-    <t>152</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX</t>
-  </si>
-  <si>
-    <t>02:37:54</t>
-  </si>
-  <si>
-    <t>Jan 29 2:08PM CST</t>
+    <t>Jan 30 3:09PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Garcia</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>02:50:14</t>
+  </si>
+  <si>
+    <t>00:01:46</t>
+  </si>
+  <si>
+    <t>00:00:45</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>Jan 30 9:06AM CST</t>
+  </si>
+  <si>
+    <t>Adrian Caro</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>FORD RANGER 2011</t>
+  </si>
+  <si>
+    <t>05:04:33</t>
+  </si>
+  <si>
+    <t>00:01:57</t>
+  </si>
+  <si>
+    <t>00:00:55</t>
+  </si>
+  <si>
+    <t>Jan 30 7:23PM CST</t>
   </si>
   <si>
     <t>Daniel Iñiguez</t>
@@ -162,31 +405,166 @@
     <t>TOYOTA HILUX 2017</t>
   </si>
   <si>
-    <t>02:30:04</t>
-  </si>
-  <si>
-    <t>00:00:05</t>
-  </si>
-  <si>
-    <t>00:00:15</t>
-  </si>
-  <si>
-    <t>Jan 29 4:40PM CST</t>
-  </si>
-  <si>
-    <t>Hugo López</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>02:32:39</t>
+    <t>04:44:10</t>
+  </si>
+  <si>
+    <t>00:01:29</t>
+  </si>
+  <si>
+    <t>00:00:23</t>
+  </si>
+  <si>
+    <t>Jan 30 2:30PM CST</t>
+  </si>
+  <si>
+    <t>Moises Martinez</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2024</t>
+  </si>
+  <si>
+    <t>03:15:54</t>
+  </si>
+  <si>
+    <t>00:03:07</t>
+  </si>
+  <si>
+    <t>00:02:04</t>
+  </si>
+  <si>
+    <t>Jan 30 1:47PM CST</t>
+  </si>
+  <si>
+    <t>Miguel Guizar</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Hino 300 2024</t>
+  </si>
+  <si>
+    <t>05:37:28</t>
+  </si>
+  <si>
+    <t>00:08:11</t>
+  </si>
+  <si>
+    <t>00:04:11</t>
+  </si>
+  <si>
+    <t>00:00:18</t>
+  </si>
+  <si>
+    <t>Jan 30 4:16PM CST</t>
+  </si>
+  <si>
+    <t>Abraham Arana</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>03:10:59</t>
+  </si>
+  <si>
+    <t>00:03:13</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>00:00:16</t>
+  </si>
+  <si>
+    <t>Jan 30 3:08PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Mercado</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>03:13:06</t>
+  </si>
+  <si>
+    <t>00:01:48</t>
+  </si>
+  <si>
+    <t>00:01:35</t>
+  </si>
+  <si>
+    <t>Jan 30 11:08AM CST</t>
+  </si>
+  <si>
+    <t>Luis Ibarra</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>03:46:49</t>
+  </si>
+  <si>
+    <t>00:01:21</t>
   </si>
   <si>
     <t>00:00:11</t>
   </si>
   <si>
-    <t>Jan 29 1:26PM CST</t>
+    <t>Jan 30 11:47AM CST</t>
+  </si>
+  <si>
+    <t>Angel Cortez</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>03:23:13</t>
+  </si>
+  <si>
+    <t>00:02:01</t>
+  </si>
+  <si>
+    <t>00:03:05</t>
+  </si>
+  <si>
+    <t>00:00:38</t>
+  </si>
+  <si>
+    <t>Jan 30 12:27PM CST</t>
+  </si>
+  <si>
+    <t>Luis Galindo</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>KENWORTH 2009</t>
+  </si>
+  <si>
+    <t>06:16:57</t>
+  </si>
+  <si>
+    <t>00:04:30</t>
+  </si>
+  <si>
+    <t>00:06:11</t>
+  </si>
+  <si>
+    <t>00:03:46</t>
+  </si>
+  <si>
+    <t>00:00:12</t>
+  </si>
+  <si>
+    <t>Jan 30 8:03AM CST</t>
   </si>
   <si>
     <t>Armando Muñoz</t>
@@ -198,61 +576,19 @@
     <t>HINO 300</t>
   </si>
   <si>
-    <t>02:18:47</t>
-  </si>
-  <si>
-    <t>00:00:16</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>Jan 29 2:56PM CST</t>
-  </si>
-  <si>
-    <t>Alejandro Suarez</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>HINO 500</t>
-  </si>
-  <si>
-    <t>02:04:50</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>Jan 29 9:52AM CST</t>
-  </si>
-  <si>
-    <t>Marcos Barbosa</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2023</t>
-  </si>
-  <si>
-    <t>02:33:33</t>
-  </si>
-  <si>
-    <t>Jan 29 3:43PM CST</t>
-  </si>
-  <si>
-    <t>Gerardo Aguillón</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>02:30:58</t>
-  </si>
-  <si>
-    <t>Jan 29 12:18PM CST</t>
+    <t>04:56:44</t>
+  </si>
+  <si>
+    <t>00:07:05</t>
+  </si>
+  <si>
+    <t>00:06:53</t>
+  </si>
+  <si>
+    <t>00:02:45</t>
+  </si>
+  <si>
+    <t>Jan 30 10:01AM CST</t>
   </si>
   <si>
     <t>Alberto Sanchez</t>
@@ -264,85 +600,67 @@
     <t>VW DELIVERY 10.6</t>
   </si>
   <si>
-    <t>00:19:48</t>
-  </si>
-  <si>
-    <t>Jan 29 3:27PM CST</t>
-  </si>
-  <si>
-    <t>Luis Galindo</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>KENWORTH 2009</t>
-  </si>
-  <si>
-    <t>00:17:50</t>
-  </si>
-  <si>
-    <t>Jan 29 3:21PM CST</t>
-  </si>
-  <si>
-    <t>Diego Cardenas</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2018</t>
-  </si>
-  <si>
-    <t>05:09:30</t>
-  </si>
-  <si>
-    <t>00:02:04</t>
-  </si>
-  <si>
-    <t>00:00:22</t>
-  </si>
-  <si>
-    <t>Jan 29 10:38AM CST</t>
-  </si>
-  <si>
-    <t>Angel Cortez</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>03:10:31</t>
-  </si>
-  <si>
-    <t>00:01:00</t>
-  </si>
-  <si>
-    <t>00:01:17</t>
-  </si>
-  <si>
-    <t>Jan 29 11:42AM CST</t>
-  </si>
-  <si>
-    <t>Luis Ibarra</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2024</t>
-  </si>
-  <si>
-    <t>03:47:39</t>
-  </si>
-  <si>
-    <t>00:00:33</t>
-  </si>
-  <si>
-    <t>00:00:54</t>
-  </si>
-  <si>
-    <t>Jan 29 2:18PM CST</t>
+    <t>08:49:03</t>
+  </si>
+  <si>
+    <t>00:11:11</t>
+  </si>
+  <si>
+    <t>00:09:43</t>
+  </si>
+  <si>
+    <t>00:06:52</t>
+  </si>
+  <si>
+    <t>00:01:06</t>
+  </si>
+  <si>
+    <t>Jan 30 6:42AM CST</t>
+  </si>
+  <si>
+    <t>Miguel Zamora</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>05:52:29</t>
+  </si>
+  <si>
+    <t>00:03:52</t>
+  </si>
+  <si>
+    <t>00:06:15</t>
+  </si>
+  <si>
+    <t>00:04:05</t>
+  </si>
+  <si>
+    <t>00:02:56</t>
+  </si>
+  <si>
+    <t>Jan 30 11:31AM CST</t>
+  </si>
+  <si>
+    <t>Emmanuel Salcedo</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>03:59:04</t>
+  </si>
+  <si>
+    <t>00:02:05</t>
+  </si>
+  <si>
+    <t>00:01:33</t>
+  </si>
+  <si>
+    <t>00:00:29</t>
+  </si>
+  <si>
+    <t>Jan 30 2:21PM CST</t>
   </si>
   <si>
     <t>Mario Ballinas</t>
@@ -351,334 +669,16 @@
     <t>144</t>
   </si>
   <si>
-    <t>02:46:56</t>
-  </si>
-  <si>
-    <t>00:00:39</t>
-  </si>
-  <si>
-    <t>00:00:20</t>
-  </si>
-  <si>
-    <t>Jan 29 1:03PM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Lopez</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2020</t>
-  </si>
-  <si>
-    <t>01:41:51</t>
-  </si>
-  <si>
-    <t>00:00:18</t>
-  </si>
-  <si>
-    <t>Jan 29 12:42PM CST</t>
-  </si>
-  <si>
-    <t>Adrian Caro</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>FORD RANGER 2011</t>
-  </si>
-  <si>
-    <t>00:54:53</t>
-  </si>
-  <si>
-    <t>Jan 29 2:42PM CST</t>
-  </si>
-  <si>
-    <t>Luis Ramirez</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>FORD F350 3MTS 2006</t>
-  </si>
-  <si>
-    <t>01:42:54</t>
-  </si>
-  <si>
-    <t>Jan 29 3:42PM CST</t>
-  </si>
-  <si>
-    <t>Daniel Mercado</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>03:17:55</t>
-  </si>
-  <si>
-    <t>00:01:23</t>
-  </si>
-  <si>
-    <t>00:02:03</t>
-  </si>
-  <si>
-    <t>Jan 29 12:52PM CST</t>
-  </si>
-  <si>
-    <t>Moises Martinez</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>03:37:52</t>
-  </si>
-  <si>
-    <t>00:01:46</t>
-  </si>
-  <si>
-    <t>00:02:27</t>
-  </si>
-  <si>
-    <t>Jan 29 3:34PM CST</t>
-  </si>
-  <si>
-    <t>José Morales</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>02:41:35</t>
-  </si>
-  <si>
-    <t>00:00:53</t>
-  </si>
-  <si>
-    <t>00:00:58</t>
-  </si>
-  <si>
-    <t>Jan 29 2:14PM CST</t>
-  </si>
-  <si>
-    <t>Abraham Arana</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>01:49:12</t>
-  </si>
-  <si>
-    <t>00:00:50</t>
-  </si>
-  <si>
-    <t>00:00:31</t>
-  </si>
-  <si>
-    <t>00:00:04</t>
-  </si>
-  <si>
-    <t>Jan 29 1:38PM CST</t>
-  </si>
-  <si>
-    <t>Miguel Guizar</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Hino 300 2024</t>
-  </si>
-  <si>
-    <t>11:13:12</t>
-  </si>
-  <si>
-    <t>00:09:31</t>
-  </si>
-  <si>
-    <t>00:05:16</t>
-  </si>
-  <si>
-    <t>00:01:42</t>
-  </si>
-  <si>
-    <t>00:00:56</t>
-  </si>
-  <si>
-    <t>Jan 29 4:47PM CST</t>
-  </si>
-  <si>
-    <t>Fernando Garcia</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
-    <t>08:34:50</t>
-  </si>
-  <si>
-    <t>00:06:05</t>
-  </si>
-  <si>
-    <t>00:09:50</t>
-  </si>
-  <si>
-    <t>00:01:40</t>
-  </si>
-  <si>
-    <t>00:00:46</t>
-  </si>
-  <si>
-    <t>Jan 29 7:16AM CST</t>
-  </si>
-  <si>
-    <t>Miguel Zamora</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>09:43:26</t>
-  </si>
-  <si>
-    <t>00:06:00</t>
-  </si>
-  <si>
-    <t>00:08:39</t>
-  </si>
-  <si>
-    <t>00:03:52</t>
-  </si>
-  <si>
-    <t>00:01:50</t>
-  </si>
-  <si>
-    <t>Jan 29 2:53AM CST</t>
-  </si>
-  <si>
-    <t>Francisco Marquez</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-  </si>
-  <si>
-    <t>05:11:04</t>
-  </si>
-  <si>
-    <t>00:03:36</t>
-  </si>
-  <si>
-    <t>00:02:39</t>
-  </si>
-  <si>
-    <t>00:05:45</t>
-  </si>
-  <si>
-    <t>00:00:49</t>
-  </si>
-  <si>
-    <t>Jan 29 12:25PM CST</t>
-  </si>
-  <si>
-    <t>Martin Quezada</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>INTERNACIONAL</t>
-  </si>
-  <si>
-    <t>05:54:37</t>
-  </si>
-  <si>
-    <t>00:06:42</t>
-  </si>
-  <si>
-    <t>00:08:32</t>
-  </si>
-  <si>
-    <t>00:04:37</t>
-  </si>
-  <si>
-    <t>00:01:49</t>
-  </si>
-  <si>
-    <t>Jan 29 2:11PM CST</t>
-  </si>
-  <si>
-    <t>Kevin De La O</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>VAN HYUNDAI</t>
-  </si>
-  <si>
-    <t>04:29:41</t>
-  </si>
-  <si>
-    <t>00:04:35</t>
-  </si>
-  <si>
-    <t>00:06:02</t>
-  </si>
-  <si>
-    <t>00:01:53</t>
-  </si>
-  <si>
-    <t>00:02:36</t>
-  </si>
-  <si>
-    <t>Fernando Ornelas</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>04:54:08</t>
-  </si>
-  <si>
-    <t>00:02:05</t>
-  </si>
-  <si>
-    <t>00:01:19</t>
-  </si>
-  <si>
-    <t>00:00:27</t>
-  </si>
-  <si>
-    <t>Jan 29 12:35PM CST</t>
-  </si>
-  <si>
-    <t>Emmanuel Salcedo</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>03:58:11</t>
-  </si>
-  <si>
-    <t>00:01:02</t>
-  </si>
-  <si>
-    <t>00:00:45</t>
-  </si>
-  <si>
-    <t>Jan 29 4:07PM CST</t>
+    <t>03:09:36</t>
+  </si>
+  <si>
+    <t>00:00:42</t>
+  </si>
+  <si>
+    <t>00:01:07</t>
+  </si>
+  <si>
+    <t>Jan 30 1:55PM CST</t>
   </si>
   <si>
     <t>Alberto Jimenez</t>
@@ -727,6 +727,9 @@
   </si>
   <si>
     <t>145</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1165,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,16 +1308,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="1">
-        <v>49.8</v>
+        <v>50.8</v>
       </c>
       <c r="G2" s="1">
-        <v>8.5</v>
+        <v>7.51</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1344,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>38</v>
@@ -1406,10 +1409,10 @@
         <v>42</v>
       </c>
       <c r="F3" s="1">
-        <v>40.700000000000003</v>
+        <v>36.6</v>
       </c>
       <c r="G3" s="1">
-        <v>5.75</v>
+        <v>6.6</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -1439,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>43</v>
@@ -1492,52 +1495,52 @@
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4.41</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>48</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F4" s="1">
-        <v>40.6</v>
-      </c>
-      <c r="G4" s="1">
-        <v>5.45</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>71.010000000000005</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -1581,31 +1584,31 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1">
-        <v>37.9</v>
+        <v>30.1</v>
       </c>
       <c r="G5" s="1">
-        <v>7.01</v>
+        <v>4.79</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>37</v>
@@ -1629,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -1676,34 +1679,34 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1">
-        <v>37.1</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1">
-        <v>4.8099999999999996</v>
+        <v>4.45</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>37</v>
@@ -1724,10 +1727,10 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1">
-        <v>69.010000000000005</v>
+        <v>52</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
@@ -1771,34 +1774,34 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2">
         <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F7" s="1">
-        <v>37.1</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G7" s="1">
-        <v>11.21</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>37</v>
@@ -1819,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1">
-        <v>65.010000000000005</v>
+        <v>52</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>
@@ -1866,25 +1869,25 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1">
-        <v>32.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G8" s="1">
-        <v>6.14</v>
+        <v>2.98</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -1914,10 +1917,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -1961,25 +1964,25 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2">
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1">
-        <v>30.9</v>
+        <v>0.2</v>
       </c>
       <c r="G9" s="1">
-        <v>5.15</v>
+        <v>1.5</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -2009,10 +2012,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -2056,25 +2059,25 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2">
         <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1">
-        <v>4.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -2104,10 +2107,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>43.83</v>
+        <v>31</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -2151,58 +2154,58 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2">
+        <v>99</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1">
+        <v>89.8</v>
+      </c>
+      <c r="G11" s="1">
+        <v>11.64</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="K11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>82.01</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="2">
-        <v>100</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4</v>
-      </c>
-      <c r="G11" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="1">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>39</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -2246,58 +2249,58 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" s="2">
         <v>99</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="1">
+        <v>83.7</v>
+      </c>
+      <c r="G12" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>73.010000000000005</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F12" s="1">
-        <v>100.7</v>
-      </c>
-      <c r="G12" s="1">
-        <v>14.4</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>71.010000000000005</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -2341,58 +2344,58 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2">
         <v>99</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="1">
+        <v>49.6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.88</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F13" s="1">
-        <v>89.7</v>
-      </c>
-      <c r="G13" s="1">
-        <v>12.04</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>79.010000000000005</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -2436,58 +2439,58 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D14" s="2">
         <v>99</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>93.19</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F14" s="1">
-        <v>83.3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>11.17</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>78.010000000000005</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -2531,34 +2534,34 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D15" s="2">
         <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F15" s="1">
-        <v>60.2</v>
+        <v>24.4</v>
       </c>
       <c r="G15" s="1">
-        <v>7.73</v>
+        <v>4.07</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>37</v>
@@ -2579,10 +2582,10 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>74.010000000000005</v>
+        <v>72.010000000000005</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2626,58 +2629,58 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="2">
+        <v>98</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="1">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="2">
-        <v>99</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="L16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>84.12</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F16" s="1">
-        <v>27</v>
-      </c>
-      <c r="G16" s="1">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>66.010000000000005</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
@@ -2721,37 +2724,37 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="2">
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="1">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1">
+        <v>12.39</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="2">
-        <v>99</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="1">
-        <v>20.3</v>
-      </c>
-      <c r="G17" s="1">
-        <v>2.48</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>37</v>
@@ -2769,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>73.010000000000005</v>
+        <v>75.010000000000005</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>124</v>
@@ -2825,28 +2828,28 @@
         <v>127</v>
       </c>
       <c r="D18" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="F18" s="1">
-        <v>19.600000000000001</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1">
-        <v>8.81</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>37</v>
@@ -2864,10 +2867,10 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1">
-        <v>62</v>
+        <v>75.010000000000005</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="S18" s="1">
         <v>0</v>
@@ -2911,37 +2914,37 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="D19" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F19" s="1">
-        <v>65</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="G19" s="1">
-        <v>9.18</v>
+        <v>11.1</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>37</v>
@@ -2962,7 +2965,7 @@
         <v>89.01</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -3006,37 +3009,37 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="D20" s="2">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F20" s="1">
-        <v>62.7</v>
+        <v>173.1</v>
       </c>
       <c r="G20" s="1">
-        <v>11.45</v>
+        <v>19.97</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>37</v>
@@ -3054,10 +3057,10 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1">
-        <v>79.010000000000005</v>
+        <v>90.01</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="S20" s="1">
         <v>0</v>
@@ -3101,37 +3104,37 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="3">
-        <v>88</v>
+        <v>41</v>
+      </c>
+      <c r="D21" s="2">
+        <v>95</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F21" s="1">
-        <v>51.3</v>
+        <v>72.8</v>
       </c>
       <c r="G21" s="1">
-        <v>6.93</v>
+        <v>9.73</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>37</v>
@@ -3149,10 +3152,10 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1">
-        <v>70.010000000000005</v>
+        <v>83.01</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -3196,40 +3199,40 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="3">
-        <v>82</v>
+        <v>127</v>
+      </c>
+      <c r="D22" s="2">
+        <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F22" s="1">
-        <v>41</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="G22" s="1">
-        <v>6.34</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>153</v>
+        <v>37</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
@@ -3244,10 +3247,10 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1">
-        <v>74.010000000000005</v>
+        <v>84.01</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="S22" s="1">
         <v>0</v>
@@ -3291,40 +3294,40 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23" s="3">
-        <v>79</v>
+        <v>134</v>
+      </c>
+      <c r="D23" s="2">
+        <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F23" s="1">
-        <v>576.6</v>
+        <v>82.8</v>
       </c>
       <c r="G23" s="1">
-        <v>77.8</v>
+        <v>10.47</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>162</v>
+        <v>56</v>
       </c>
       <c r="M23" s="1">
         <v>0</v>
@@ -3339,10 +3342,10 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>106.01</v>
+        <v>64</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="S23" s="1">
         <v>0</v>
@@ -3386,46 +3389,46 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="D24" s="3">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F24" s="1">
-        <v>490.3</v>
+        <v>118.1</v>
       </c>
       <c r="G24" s="1">
-        <v>0</v>
+        <v>14.19</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>171</v>
+        <v>35</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1">
         <v>0</v>
@@ -3434,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>99.11</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>172</v>
@@ -3487,40 +3490,40 @@
         <v>174</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D25" s="4">
-        <v>54</v>
+        <v>175</v>
+      </c>
+      <c r="D25" s="3">
+        <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F25" s="1">
-        <v>410.7</v>
+        <v>332.3</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>80.260000000000005</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -3529,10 +3532,10 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1">
-        <v>105.5</v>
+        <v>93.01</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="S25" s="1">
         <v>0</v>
@@ -3576,55 +3579,55 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D26" s="4">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F26" s="1">
-        <v>307.8</v>
+        <v>249.7</v>
       </c>
       <c r="G26" s="1">
-        <v>82</v>
+        <v>32.270000000000003</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>188</v>
+        <v>108</v>
       </c>
       <c r="M26" s="1">
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" s="1">
         <v>0</v>
       </c>
       <c r="Q26" s="1">
-        <v>95.01</v>
+        <v>92.01</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>189</v>
@@ -3680,16 +3683,16 @@
         <v>192</v>
       </c>
       <c r="D27" s="4">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>193</v>
       </c>
       <c r="F27" s="1">
-        <v>325.3</v>
-      </c>
-      <c r="G27" s="1">
-        <v>117.93</v>
+        <v>349.4</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="H27" s="1">
         <v>1</v>
@@ -3710,16 +3713,16 @@
         <v>0</v>
       </c>
       <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
         <v>2</v>
       </c>
-      <c r="O27" s="1">
-        <v>1</v>
-      </c>
       <c r="P27" s="1">
         <v>0</v>
       </c>
       <c r="Q27" s="1">
-        <v>102.01</v>
+        <v>95.53</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>198</v>
@@ -3728,13 +3731,13 @@
         <v>0</v>
       </c>
       <c r="T27" s="1">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
         <v>1</v>
-      </c>
-      <c r="U27" s="1">
-        <v>0</v>
-      </c>
-      <c r="V27" s="1">
-        <v>0</v>
       </c>
       <c r="W27" s="1">
         <v>0</v>
@@ -3772,34 +3775,34 @@
         <v>200</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1">
+        <v>299.89999999999998</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F28" s="1">
-        <v>154.30000000000001</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
@@ -3814,10 +3817,10 @@
         <v>1</v>
       </c>
       <c r="Q28" s="1">
-        <v>109.03</v>
+        <v>104.78</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>50</v>
+        <v>206</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -3867,7 +3870,7 @@
         <v>208</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -3876,13 +3879,13 @@
         <v>209</v>
       </c>
       <c r="F29" s="1">
-        <v>86.8</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="G29" s="1">
-        <v>15.6</v>
+        <v>14.57</v>
       </c>
       <c r="H29" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>210</v>
@@ -3894,7 +3897,7 @@
         <v>212</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="M29" s="1">
         <v>0</v>
@@ -3909,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1">
-        <v>73.010000000000005</v>
+        <v>100.01</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>213</v>
@@ -3918,13 +3921,13 @@
         <v>0</v>
       </c>
       <c r="T29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" s="1">
         <v>0</v>
       </c>
       <c r="V29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W29" s="1">
         <v>0</v>
@@ -3945,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="AC29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD29" s="1">
         <v>0</v>
@@ -3962,22 +3965,22 @@
         <v>215</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D30" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>216</v>
       </c>
       <c r="F30" s="1">
-        <v>69.5</v>
+        <v>65.2</v>
       </c>
       <c r="G30" s="1">
-        <v>14.02</v>
+        <v>9.39</v>
       </c>
       <c r="H30" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>217</v>
@@ -3986,10 +3989,10 @@
         <v>218</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="M30" s="1">
         <v>0</v>
@@ -4004,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1">
-        <v>83.01</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>219</v>
@@ -4019,13 +4022,13 @@
         <v>0</v>
       </c>
       <c r="V30" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W30" s="1">
         <v>0</v>
       </c>
       <c r="X30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y30" s="1" t="s">
         <v>37</v>
@@ -4057,7 +4060,7 @@
         <v>221</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>201</v>
+        <v>100</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>222</v>
@@ -4342,7 +4345,7 @@
         <v>230</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>222</v>
@@ -4532,7 +4535,7 @@
         <v>235</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
Actualización de archivos en la carpeta data - 2025-02-06 09:17:23
</commit_message>
<xml_diff>
--- a/data/Informe_Diario_Unidades.xlsx
+++ b/data/Informe_Diario_Unidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="232">
   <si>
     <t>Operador</t>
   </si>
@@ -114,28 +114,229 @@
     <t>Comer/Beber (Manual)</t>
   </si>
   <si>
+    <t>Diego Cardenas</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2018</t>
+  </si>
+  <si>
+    <t>04:53:38</t>
+  </si>
+  <si>
+    <t>00:00:40</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>Feb 5 5:02PM CST</t>
+  </si>
+  <si>
+    <t>Luis Ibarra</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2024</t>
+  </si>
+  <si>
+    <t>04:09:11</t>
+  </si>
+  <si>
+    <t>00:00:17</t>
+  </si>
+  <si>
+    <t>Feb 5 1:29PM CST</t>
+  </si>
+  <si>
+    <t>Christian Aguilar</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2021</t>
+  </si>
+  <si>
+    <t>02:55:42</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>Feb 5 11:28AM CST</t>
+  </si>
+  <si>
+    <t>Gerardo Aguillón</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>02:18:43</t>
+  </si>
+  <si>
+    <t>Feb 5 8:06AM CST</t>
+  </si>
+  <si>
+    <t>Marcos Barbosa</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2023</t>
+  </si>
+  <si>
+    <t>01:59:38</t>
+  </si>
+  <si>
+    <t>Feb 5 1:55PM CST</t>
+  </si>
+  <si>
+    <t>Luis Ramirez</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>FORD F350 3MTS 2006</t>
+  </si>
+  <si>
+    <t>01:46:56</t>
+  </si>
+  <si>
+    <t>Feb 5 8:35AM CST</t>
+  </si>
+  <si>
+    <t>Luis Galindo</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>KENWORTH 2009</t>
+  </si>
+  <si>
+    <t>00:01:15</t>
+  </si>
+  <si>
+    <t>Feb 5 8:29PM CST</t>
+  </si>
+  <si>
+    <t>Alejandro Suarez</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>HINO 500</t>
+  </si>
+  <si>
+    <t>00:00:49</t>
+  </si>
+  <si>
+    <t>Feb 5 5:53PM CST</t>
+  </si>
+  <si>
     <t>Angel Cortez</t>
   </si>
   <si>
     <t>133</t>
   </si>
   <si>
-    <t>TOYOTA HILUX 2018</t>
-  </si>
-  <si>
-    <t>02:59:41</t>
+    <t>03:20:31</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>00:00:21</t>
+  </si>
+  <si>
+    <t>Feb 5 11:51AM CST</t>
+  </si>
+  <si>
+    <t>Moises Martinez</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>02:37:03</t>
+  </si>
+  <si>
+    <t>00:00:59</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
+    <t>Feb 5 2:12PM CST</t>
+  </si>
+  <si>
+    <t>Eduardo Hernandez</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX</t>
+  </si>
+  <si>
+    <t>02:56:33</t>
   </si>
   <si>
     <t>00:00:32</t>
   </si>
   <si>
-    <t>00:00:04</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
-    <t>Feb 4 3:04PM CST</t>
+    <t>Feb 5 3:10PM CST</t>
+  </si>
+  <si>
+    <t>José Morales</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>01:45:17</t>
+  </si>
+  <si>
+    <t>00:01:06</t>
+  </si>
+  <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
+    <t>Feb 5 1:20PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Ornelas</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2020</t>
+  </si>
+  <si>
+    <t>02:10:14</t>
+  </si>
+  <si>
+    <t>00:00:36</t>
+  </si>
+  <si>
+    <t>00:00:56</t>
+  </si>
+  <si>
+    <t>Feb 5 2:02PM CST</t>
   </si>
   <si>
     <t>Hugo López</t>
@@ -144,61 +345,85 @@
     <t>153</t>
   </si>
   <si>
-    <t>TOYOTA HILUX</t>
-  </si>
-  <si>
-    <t>02:32:36</t>
-  </si>
-  <si>
-    <t>00:00:27</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>Feb 4 2:13PM CST</t>
-  </si>
-  <si>
-    <t>Christian Aguilar</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2021</t>
-  </si>
-  <si>
-    <t>02:54:30</t>
-  </si>
-  <si>
-    <t>Feb 4 2:49PM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Hernandez</t>
-  </si>
-  <si>
-    <t>152</t>
-  </si>
-  <si>
-    <t>02:19:39</t>
-  </si>
-  <si>
-    <t>00:00:05</t>
-  </si>
-  <si>
-    <t>Feb 4 2:31PM CST</t>
-  </si>
-  <si>
-    <t>Gerardo Aguillón</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>02:44:28</t>
-  </si>
-  <si>
-    <t>Feb 4 5:23PM CST</t>
+    <t>02:37:13</t>
+  </si>
+  <si>
+    <t>00:00:15</t>
+  </si>
+  <si>
+    <t>Feb 5 3:07PM CST</t>
+  </si>
+  <si>
+    <t>Mario Ballinas</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>00:49:58</t>
+  </si>
+  <si>
+    <t>Feb 5 2:23PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Iñiguez</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2017</t>
+  </si>
+  <si>
+    <t>04:03:53</t>
+  </si>
+  <si>
+    <t>00:01:38</t>
+  </si>
+  <si>
+    <t>Feb 5 9:49AM CST</t>
+  </si>
+  <si>
+    <t>Daniel Mercado</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>04:31:59</t>
+  </si>
+  <si>
+    <t>00:04:19</t>
+  </si>
+  <si>
+    <t>00:06:27</t>
+  </si>
+  <si>
+    <t>Feb 5 12:41PM CST</t>
+  </si>
+  <si>
+    <t>Francisco Marquez</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+  </si>
+  <si>
+    <t>09:37:05</t>
+  </si>
+  <si>
+    <t>00:07:41</t>
+  </si>
+  <si>
+    <t>00:06:10</t>
+  </si>
+  <si>
+    <t>00:01:59</t>
+  </si>
+  <si>
+    <t>Feb 5 10:56AM CST</t>
   </si>
   <si>
     <t>Eduardo Lopez</t>
@@ -207,34 +432,124 @@
     <t>136</t>
   </si>
   <si>
-    <t>TOYOTA HILUX 2020</t>
-  </si>
-  <si>
-    <t>02:09:29</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>00:00:17</t>
-  </si>
-  <si>
-    <t>Feb 4 12:21PM CST</t>
-  </si>
-  <si>
-    <t>Marcos Barbosa</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2023</t>
-  </si>
-  <si>
-    <t>01:35:30</t>
-  </si>
-  <si>
-    <t>Feb 4 1:14PM CST</t>
+    <t>02:53:21</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>00:00:39</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>Feb 5 4:31PM CST</t>
+  </si>
+  <si>
+    <t>Martin Quezada</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>05:20:53</t>
+  </si>
+  <si>
+    <t>00:05:54</t>
+  </si>
+  <si>
+    <t>00:05:15</t>
+  </si>
+  <si>
+    <t>00:05:21</t>
+  </si>
+  <si>
+    <t>Feb 5 1:32PM CST</t>
+  </si>
+  <si>
+    <t>Miguel Guizar</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Hino 300 2024</t>
+  </si>
+  <si>
+    <t>08:38:02</t>
+  </si>
+  <si>
+    <t>00:07:28</t>
+  </si>
+  <si>
+    <t>00:04:11</t>
+  </si>
+  <si>
+    <t>00:01:42</t>
+  </si>
+  <si>
+    <t>00:02:07</t>
+  </si>
+  <si>
+    <t>Feb 5 1:51PM CST</t>
+  </si>
+  <si>
+    <t>Alberto Sanchez</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>VW DELIVERY 10.6</t>
+  </si>
+  <si>
+    <t>07:58:09</t>
+  </si>
+  <si>
+    <t>00:15:47</t>
+  </si>
+  <si>
+    <t>00:11:44</t>
+  </si>
+  <si>
+    <t>00:04:46</t>
+  </si>
+  <si>
+    <t>00:01:32</t>
+  </si>
+  <si>
+    <t>Feb 5 3:00PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Garcia</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>06:14:52</t>
+  </si>
+  <si>
+    <t>00:06:51</t>
+  </si>
+  <si>
+    <t>00:03:12</t>
+  </si>
+  <si>
+    <t>00:04:56</t>
+  </si>
+  <si>
+    <t>00:02:10</t>
+  </si>
+  <si>
+    <t>Feb 5 11:15AM CST</t>
   </si>
   <si>
     <t>Miguel Zamora</t>
@@ -243,13 +558,43 @@
     <t>139</t>
   </si>
   <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
-    <t>01:09:15</t>
-  </si>
-  <si>
-    <t>Feb 4 3:44PM CST</t>
+    <t>11:21:38</t>
+  </si>
+  <si>
+    <t>00:14:17</t>
+  </si>
+  <si>
+    <t>00:17:37</t>
+  </si>
+  <si>
+    <t>00:11:30</t>
+  </si>
+  <si>
+    <t>Feb 5 8:25AM CST</t>
+  </si>
+  <si>
+    <t>Jorge Tornero</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>HINO 300</t>
+  </si>
+  <si>
+    <t>05:00:23</t>
+  </si>
+  <si>
+    <t>00:03:25</t>
+  </si>
+  <si>
+    <t>00:04:35</t>
+  </si>
+  <si>
+    <t>00:00:34</t>
+  </si>
+  <si>
+    <t>Feb 5 1:13PM CST</t>
   </si>
   <si>
     <t>Armando Muñoz</t>
@@ -258,451 +603,115 @@
     <t>102</t>
   </si>
   <si>
-    <t>HINO 300</t>
-  </si>
-  <si>
-    <t>00:37:19</t>
-  </si>
-  <si>
-    <t>Feb 4 2:14PM CST</t>
-  </si>
-  <si>
-    <t>Jorge Tornero</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>00:15:55</t>
-  </si>
-  <si>
-    <t>Feb 4 6:00PM CST</t>
-  </si>
-  <si>
-    <t>Alejandro Suarez</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>HINO 500</t>
-  </si>
-  <si>
-    <t>00:21:26</t>
-  </si>
-  <si>
-    <t>Feb 4 1:32PM CST</t>
-  </si>
-  <si>
-    <t>Francisco Marquez</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-  </si>
-  <si>
-    <t>00:01:38</t>
-  </si>
-  <si>
-    <t>Feb 4 6:37PM CST</t>
-  </si>
-  <si>
-    <t>Diego Cardenas</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>01:40:13</t>
-  </si>
-  <si>
-    <t>00:00:42</t>
-  </si>
-  <si>
-    <t>Feb 4 3:12PM CST</t>
-  </si>
-  <si>
-    <t>Luis Ramirez</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>FORD F350 3MTS 2006</t>
-  </si>
-  <si>
-    <t>03:08:03</t>
-  </si>
-  <si>
-    <t>00:01:51</t>
-  </si>
-  <si>
-    <t>00:01:00</t>
-  </si>
-  <si>
-    <t>Feb 4 12:29PM CST</t>
-  </si>
-  <si>
-    <t>Daniel Mercado</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2017</t>
-  </si>
-  <si>
-    <t>03:16:03</t>
-  </si>
-  <si>
-    <t>00:01:08</t>
+    <t>05:16:53</t>
+  </si>
+  <si>
+    <t>00:02:37</t>
+  </si>
+  <si>
+    <t>00:01:07</t>
+  </si>
+  <si>
+    <t>Feb 5 11:25AM CST</t>
+  </si>
+  <si>
+    <t>Abraham Arana</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>02:40:16</t>
+  </si>
+  <si>
+    <t>00:01:23</t>
+  </si>
+  <si>
+    <t>00:01:14</t>
+  </si>
+  <si>
+    <t>00:00:26</t>
+  </si>
+  <si>
+    <t>Feb 5 4:01PM CST</t>
+  </si>
+  <si>
+    <t>Emmanuel Salcedo</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>02:41:45</t>
+  </si>
+  <si>
+    <t>00:01:11</t>
   </si>
   <si>
     <t>00:00:16</t>
   </si>
   <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>Feb 4 12:49AM CST</t>
+    <t>Feb 5 1:58PM CST</t>
+  </si>
+  <si>
+    <t>Alberto Jimenez</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>VAN HYUNDAI</t>
+  </si>
+  <si>
+    <t>Sin ruta</t>
+  </si>
+  <si>
+    <t>Alejandro Lara</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>WORKEN</t>
+  </si>
+  <si>
+    <t>Alberto Compras</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>NISSAN 1993</t>
+  </si>
+  <si>
+    <t>Kevin De La O</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>Adrian Caro</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>FORD RANGER 2011</t>
+  </si>
+  <si>
+    <t>Álvaro Zapata</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>KENWORTH</t>
   </si>
   <si>
     <t>Alexis Alvarado</t>
   </si>
   <si>
     <t>145</t>
-  </si>
-  <si>
-    <t>00:24:20</t>
-  </si>
-  <si>
-    <t>Feb 4 4:52PM CST</t>
-  </si>
-  <si>
-    <t>Miguel Guizar</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Hino 300 2024</t>
-  </si>
-  <si>
-    <t>09:47:50</t>
-  </si>
-  <si>
-    <t>00:08:07</t>
-  </si>
-  <si>
-    <t>00:05:56</t>
-  </si>
-  <si>
-    <t>Feb 4 5:04PM CST</t>
-  </si>
-  <si>
-    <t>Abraham Arana</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>04:01:07</t>
-  </si>
-  <si>
-    <t>00:02:18</t>
-  </si>
-  <si>
-    <t>00:02:19</t>
-  </si>
-  <si>
-    <t>Feb 4 11:31AM CST</t>
-  </si>
-  <si>
-    <t>Fernando Ornelas</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>02:11:48</t>
-  </si>
-  <si>
-    <t>00:01:27</t>
-  </si>
-  <si>
-    <t>00:01:56</t>
-  </si>
-  <si>
-    <t>Feb 4 11:34AM CST</t>
-  </si>
-  <si>
-    <t>Daniel Iñiguez</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>05:48:54</t>
-  </si>
-  <si>
-    <t>00:02:47</t>
-  </si>
-  <si>
-    <t>00:02:00</t>
-  </si>
-  <si>
-    <t>00:00:26</t>
-  </si>
-  <si>
-    <t>Feb 4 3:21PM CST</t>
-  </si>
-  <si>
-    <t>José Morales</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>02:57:22</t>
-  </si>
-  <si>
-    <t>00:02:16</t>
-  </si>
-  <si>
-    <t>Feb 4 2:35PM CST</t>
-  </si>
-  <si>
-    <t>Luis Ibarra</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2024</t>
-  </si>
-  <si>
-    <t>03:00:06</t>
-  </si>
-  <si>
-    <t>00:00:20</t>
-  </si>
-  <si>
-    <t>Feb 4 4:21PM CST</t>
-  </si>
-  <si>
-    <t>Moises Martinez</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>02:58:37</t>
-  </si>
-  <si>
-    <t>00:01:24</t>
-  </si>
-  <si>
-    <t>00:00:23</t>
-  </si>
-  <si>
-    <t>Feb 4 4:50PM CST</t>
-  </si>
-  <si>
-    <t>Mario Ballinas</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>02:17:11</t>
-  </si>
-  <si>
-    <t>00:02:10</t>
-  </si>
-  <si>
-    <t>00:01:45</t>
-  </si>
-  <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>Feb 4 3:39PM CST</t>
-  </si>
-  <si>
-    <t>Martin Quezada</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>INTERNACIONAL</t>
-  </si>
-  <si>
-    <t>09:06:21</t>
-  </si>
-  <si>
-    <t>00:04:30</t>
-  </si>
-  <si>
-    <t>00:09:27</t>
-  </si>
-  <si>
-    <t>00:03:28</t>
-  </si>
-  <si>
-    <t>00:00:36</t>
-  </si>
-  <si>
-    <t>Feb 4 6:18AM CST</t>
-  </si>
-  <si>
-    <t>Fernando Garcia</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>09:34:51</t>
-  </si>
-  <si>
-    <t>00:06:46</t>
-  </si>
-  <si>
-    <t>00:10:13</t>
-  </si>
-  <si>
-    <t>00:06:55</t>
-  </si>
-  <si>
-    <t>Feb 4 3:19AM CST</t>
-  </si>
-  <si>
-    <t>Luis Galindo</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>KENWORTH 2009</t>
-  </si>
-  <si>
-    <t>09:29:47</t>
-  </si>
-  <si>
-    <t>00:04:39</t>
-  </si>
-  <si>
-    <t>00:11:06</t>
-  </si>
-  <si>
-    <t>00:05:28</t>
-  </si>
-  <si>
-    <t>Feb 4 11:57AM CST</t>
-  </si>
-  <si>
-    <t>Alberto Sanchez</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>VW DELIVERY 10.6</t>
-  </si>
-  <si>
-    <t>09:10:17</t>
-  </si>
-  <si>
-    <t>00:10:25</t>
-  </si>
-  <si>
-    <t>00:14:47</t>
-  </si>
-  <si>
-    <t>00:08:44</t>
-  </si>
-  <si>
-    <t>00:08:28</t>
-  </si>
-  <si>
-    <t>Feb 4 1:15PM CST</t>
-  </si>
-  <si>
-    <t>Emmanuel Salcedo</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>03:13:41</t>
-  </si>
-  <si>
-    <t>00:01:11</t>
-  </si>
-  <si>
-    <t>00:00:49</t>
-  </si>
-  <si>
-    <t>00:00:15</t>
-  </si>
-  <si>
-    <t>Feb 4 5:17PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Jimenez</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>VAN HYUNDAI</t>
-  </si>
-  <si>
-    <t>Sin ruta</t>
-  </si>
-  <si>
-    <t>Alejandro Lara</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>WORKEN</t>
-  </si>
-  <si>
-    <t>Alberto Compras</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>NISSAN 1993</t>
-  </si>
-  <si>
-    <t>Kevin De La O</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>Adrian Caro</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>FORD RANGER 2011</t>
-  </si>
-  <si>
-    <t>Álvaro Zapata</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>KENWORTH</t>
   </si>
   <si>
     <t>/</t>
@@ -731,7 +740,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,12 +751,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF92D050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -775,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,13 +786,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1141,7 +1141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G29" sqref="G29"/>
+      <selection pane="topRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,10 +1290,10 @@
         <v>34</v>
       </c>
       <c r="F2" s="1">
-        <v>92.1</v>
+        <v>102.5</v>
       </c>
       <c r="G2" s="1">
-        <v>13.14</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>82.01</v>
+        <v>75.010000000000005</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>38</v>
@@ -1385,10 +1385,10 @@
         <v>42</v>
       </c>
       <c r="F3" s="1">
-        <v>43.3</v>
+        <v>79.7</v>
       </c>
       <c r="G3" s="1">
-        <v>8.17</v>
+        <v>12.37</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -1397,31 +1397,31 @@
         <v>43</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>66.010000000000005</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>62</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
@@ -1465,32 +1465,32 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="1">
-        <v>39.5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>6.94</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>50</v>
@@ -1566,7 +1566,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
@@ -1575,43 +1575,43 @@
         <v>53</v>
       </c>
       <c r="F5" s="1">
-        <v>38.6</v>
+        <v>28.5</v>
       </c>
       <c r="G5" s="1">
-        <v>5.47</v>
+        <v>4.43</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>42</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>60</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -1670,10 +1670,10 @@
         <v>58</v>
       </c>
       <c r="F6" s="1">
-        <v>36.9</v>
+        <v>26.1</v>
       </c>
       <c r="G6" s="1">
-        <v>5.96</v>
+        <v>3.99</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>59</v>
@@ -1765,43 +1765,43 @@
         <v>63</v>
       </c>
       <c r="F7" s="1">
-        <v>34.6</v>
+        <v>19.2</v>
       </c>
       <c r="G7" s="1">
-        <v>6.44</v>
+        <v>7.38</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>49</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>67.010000000000005</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>
@@ -1845,25 +1845,25 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1">
-        <v>20.100000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G8" s="1">
-        <v>2.86</v>
+        <v>0.49</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -1893,10 +1893,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -1940,31 +1940,31 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D9" s="2">
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" s="1">
-        <v>13.4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>228</v>
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.42</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>37</v>
@@ -1988,10 +1988,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1">
-        <v>63.29</v>
+        <v>26</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -2035,58 +2035,58 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2">
+        <v>99</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="1">
+        <v>96.5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>13.79</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="2">
-        <v>100</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="K10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>78.010000000000005</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="1">
-        <v>9.6</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>65.010000000000005</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -2130,34 +2130,34 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2">
+        <v>99</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="2">
-        <v>100</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1">
+        <v>62.9</v>
+      </c>
+      <c r="G11" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="1">
-        <v>5.3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>37</v>
@@ -2178,10 +2178,10 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1">
-        <v>67.010000000000005</v>
+        <v>82.01</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -2225,34 +2225,34 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D12" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1">
-        <v>4.0999999999999996</v>
+        <v>43.3</v>
       </c>
       <c r="G12" s="1">
-        <v>1.64</v>
+        <v>6.5</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>37</v>
@@ -2273,10 +2273,10 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -2320,34 +2320,34 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F13" s="1">
-        <v>0.2</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="G13" s="1">
-        <v>0.5</v>
+        <v>4.92</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>37</v>
@@ -2368,10 +2368,10 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>16</v>
+        <v>71.010000000000005</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -2415,34 +2415,34 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="D14" s="2">
         <v>99</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F14" s="1">
-        <v>25.7</v>
+        <v>36.9</v>
       </c>
       <c r="G14" s="1">
-        <v>3.52</v>
+        <v>6.42</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>37</v>
@@ -2463,10 +2463,10 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1">
-        <v>63</v>
+        <v>83.01</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -2510,34 +2510,34 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F15" s="1">
-        <v>80.8</v>
+        <v>34.5</v>
       </c>
       <c r="G15" s="1">
-        <v>18.23</v>
+        <v>6.94</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>37</v>
@@ -2558,10 +2558,10 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>77.010000000000005</v>
+        <v>63</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2605,58 +2605,58 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="2">
+        <v>99</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="1">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2.44</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="2">
-        <v>98</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16" s="1">
-        <v>80.8</v>
-      </c>
-      <c r="G16" s="1">
-        <v>11.11</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="J16" s="1" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>59</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>79.010000000000005</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
@@ -2700,37 +2700,37 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="D17" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>118</v>
       </c>
       <c r="F17" s="1">
-        <v>9.6</v>
+        <v>72.5</v>
       </c>
       <c r="G17" s="1">
-        <v>2.68</v>
+        <v>11.07</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>37</v>
@@ -2748,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>64</v>
+        <v>71.010000000000005</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S17" s="1">
         <v>0</v>
@@ -2795,25 +2795,25 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D18" s="2">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F18" s="1">
-        <v>453.7</v>
+        <v>133.30000000000001</v>
       </c>
       <c r="G18" s="1">
-        <v>55.87</v>
+        <v>16.690000000000001</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -2825,7 +2825,7 @@
         <v>125</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>37</v>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O18" s="1">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1">
-        <v>111.01</v>
+        <v>84.01</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>126</v>
@@ -2896,40 +2896,40 @@
         <v>128</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="D19" s="2">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F19" s="1">
-        <v>99.8</v>
+        <v>625.20000000000005</v>
       </c>
       <c r="G19" s="1">
-        <v>12.86</v>
+        <v>188.49</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="1">
         <v>0</v>
@@ -2938,10 +2938,10 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1">
-        <v>84.01</v>
+        <v>96.01</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -2985,37 +2985,37 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F20" s="1">
-        <v>43.3</v>
+        <v>57.5</v>
       </c>
       <c r="G20" s="1">
-        <v>6.77</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>37</v>
@@ -3033,10 +3033,10 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1">
-        <v>76.010000000000005</v>
+        <v>83.01</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="S20" s="1">
         <v>0</v>
@@ -3080,40 +3080,40 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="2">
-        <v>96</v>
+        <v>144</v>
+      </c>
+      <c r="D21" s="3">
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F21" s="1">
-        <v>132.6</v>
+        <v>319.8</v>
       </c>
       <c r="G21" s="1">
-        <v>15.56</v>
+        <v>41.84</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="M21" s="1">
         <v>0</v>
@@ -3122,16 +3122,16 @@
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21" s="1">
-        <v>75.010000000000005</v>
+        <v>101.01</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -3175,40 +3175,40 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="2">
-        <v>96</v>
+        <v>152</v>
+      </c>
+      <c r="D22" s="3">
+        <v>51</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F22" s="1">
-        <v>82.6</v>
+        <v>490.9</v>
       </c>
       <c r="G22" s="1">
-        <v>9.23</v>
+        <v>61.54</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
@@ -3223,10 +3223,10 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1">
-        <v>83.01</v>
+        <v>107.01</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="S22" s="1">
         <v>0</v>
@@ -3270,46 +3270,46 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="2">
-        <v>95</v>
+        <v>161</v>
+      </c>
+      <c r="D23" s="3">
+        <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F23" s="1">
-        <v>83.5</v>
-      </c>
-      <c r="G23" s="1">
-        <v>10.58</v>
+        <v>520.70000000000005</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="M23" s="1">
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="1">
         <v>0</v>
@@ -3318,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>80.010000000000005</v>
+        <v>97.61</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="S23" s="1">
         <v>0</v>
@@ -3365,40 +3365,40 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="2">
-        <v>95</v>
+        <v>170</v>
+      </c>
+      <c r="D24" s="3">
+        <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="F24" s="1">
-        <v>63.2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>9.5500000000000007</v>
+        <v>343.3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
@@ -3413,10 +3413,10 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>80.010000000000005</v>
+        <v>98.93</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="S24" s="1">
         <v>0</v>
@@ -3460,58 +3460,58 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>170</v>
       </c>
       <c r="D25" s="3">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="F25" s="1">
-        <v>51.6</v>
-      </c>
-      <c r="G25" s="1">
-        <v>6.46</v>
+        <v>666</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>54</v>
+        <v>182</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
       </c>
       <c r="P25" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="1">
-        <v>80.010000000000005</v>
+        <v>105.8</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="S25" s="1">
         <v>0</v>
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y25" s="1" t="s">
         <v>37</v>
@@ -3555,43 +3555,43 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="D26" s="3">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F26" s="1">
-        <v>425.2</v>
+        <v>102.9</v>
       </c>
       <c r="G26" s="1">
-        <v>172.91</v>
+        <v>9.9</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>177</v>
+        <v>36</v>
       </c>
       <c r="M26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1">
         <v>1</v>
@@ -3603,10 +3603,10 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1">
-        <v>101.01</v>
+        <v>74.010000000000005</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="S26" s="1">
         <v>0</v>
@@ -3639,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD26" s="1">
         <v>0</v>
@@ -3650,64 +3650,64 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="D27" s="3">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F27" s="1">
-        <v>405.3</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>228</v>
+        <v>100.8</v>
+      </c>
+      <c r="G27" s="1">
+        <v>12.3</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>184</v>
+        <v>37</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>168</v>
+        <v>37</v>
       </c>
       <c r="M27" s="1">
         <v>0</v>
       </c>
       <c r="N27" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O27" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P27" s="1">
         <v>0</v>
       </c>
       <c r="Q27" s="1">
-        <v>97.2</v>
+        <v>69.010000000000005</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
       </c>
       <c r="T27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27" s="1">
         <v>0</v>
@@ -3745,70 +3745,70 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D28" s="4">
-        <v>65</v>
+        <v>47</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="F28" s="1">
-        <v>585</v>
+        <v>49.5</v>
       </c>
       <c r="G28" s="1">
-        <v>161.72999999999999</v>
+        <v>7.89</v>
       </c>
       <c r="H28" s="1">
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>161</v>
+        <v>37</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O28" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
       </c>
       <c r="Q28" s="1">
-        <v>97.01</v>
+        <v>84.01</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
       </c>
       <c r="T28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="1">
         <v>0</v>
       </c>
       <c r="V28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28" s="1">
         <v>0</v>
@@ -3840,76 +3840,76 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D29" s="4">
+        <v>117</v>
+      </c>
+      <c r="D29" s="3">
         <v>0</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F29" s="1">
-        <v>595.5</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>228</v>
+        <v>44.1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>8.4</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>199</v>
+        <v>35</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
       <c r="M29" s="1">
         <v>0</v>
       </c>
       <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>77.010000000000005</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0</v>
+      </c>
+      <c r="X29" s="1">
         <v>1</v>
-      </c>
-      <c r="O29" s="1">
-        <v>1</v>
-      </c>
-      <c r="P29" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>97.96</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S29" s="1">
-        <v>0</v>
-      </c>
-      <c r="T29" s="1">
-        <v>0</v>
-      </c>
-      <c r="U29" s="1">
-        <v>0</v>
-      </c>
-      <c r="V29" s="1">
-        <v>0</v>
-      </c>
-      <c r="W29" s="1">
-        <v>0</v>
-      </c>
-      <c r="X29" s="1">
-        <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>37</v>
@@ -3935,667 +3935,667 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F30" s="1">
-        <v>75.8</v>
-      </c>
-      <c r="G30" s="1">
-        <v>11.6</v>
-      </c>
-      <c r="H30" s="1">
-        <v>2</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M30" s="1">
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>90.01</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="S30" s="1">
-        <v>0</v>
-      </c>
-      <c r="T30" s="1">
-        <v>0</v>
-      </c>
-      <c r="U30" s="1">
-        <v>0</v>
-      </c>
-      <c r="V30" s="1">
-        <v>0</v>
-      </c>
-      <c r="W30" s="1">
-        <v>0</v>
-      </c>
-      <c r="X30" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="1">
-        <v>2</v>
-      </c>
-      <c r="AD30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE30" s="1">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE30" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD31" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE31" s="6" t="s">
-        <v>213</v>
+        <v>217</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD31" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE31" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD32" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE32" s="6" t="s">
-        <v>213</v>
+        <v>220</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D33" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD33" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE33" s="6" t="s">
-        <v>213</v>
+      <c r="D33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD33" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE33" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE34" s="6" t="s">
-        <v>213</v>
+        <v>225</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD34" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE34" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE35" s="6" t="s">
-        <v>213</v>
+        <v>228</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE35" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="M36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="N36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="P36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="R36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="S36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="T36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="U36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="V36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AC36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD36" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE36" s="6" t="s">
-        <v>213</v>
+        <v>72</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD36" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE36" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de archivos en la carpeta data - 2025-03-29 08:10:04
</commit_message>
<xml_diff>
--- a/data/Informe_Diario_Unidades.xlsx
+++ b/data/Informe_Diario_Unidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="243">
   <si>
     <t>Operador</t>
   </si>
@@ -114,148 +114,484 @@
     <t>Comer/Beber (Manual)</t>
   </si>
   <si>
+    <t>Miguel Guizar</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Hino 300 2024</t>
+  </si>
+  <si>
+    <t>04:44:30</t>
+  </si>
+  <si>
+    <t>00:00:41</t>
+  </si>
+  <si>
+    <t>00:00:27</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>Mar 27 4:47PM CST</t>
+  </si>
+  <si>
+    <t>Eduardo Hernandez</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX</t>
+  </si>
+  <si>
+    <t>03:22:13</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>Mar 27 10:11AM CST</t>
+  </si>
+  <si>
+    <t>Luis Ibarra</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2024</t>
+  </si>
+  <si>
+    <t>02:27:49</t>
+  </si>
+  <si>
+    <t>Mar 27 9:28AM CST</t>
+  </si>
+  <si>
+    <t>Kevin De La O</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>VAN HYUNDAI</t>
+  </si>
+  <si>
+    <t>01:10:01</t>
+  </si>
+  <si>
+    <t>Mar 27 3:28AM CST</t>
+  </si>
+  <si>
+    <t>Christian Aguilar</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2021</t>
+  </si>
+  <si>
+    <t>03:15:10</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>Mar 27 10:25AM CST</t>
+  </si>
+  <si>
+    <t>Francisco Marquez</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+  </si>
+  <si>
+    <t>01:24:21</t>
+  </si>
+  <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
+    <t>Mar 27 1:06PM CST</t>
+  </si>
+  <si>
+    <t>Gerardo Aguillón</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>02:45:17</t>
+  </si>
+  <si>
+    <t>Mar 27 1:55PM CST</t>
+  </si>
+  <si>
+    <t>Marcos Barbosa</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2023</t>
+  </si>
+  <si>
+    <t>02:36:50</t>
+  </si>
+  <si>
+    <t>Mar 27 1:23PM CST</t>
+  </si>
+  <si>
+    <t>Hugo López</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>02:05:56</t>
+  </si>
+  <si>
+    <t>Mar 27 9:10AM CST</t>
+  </si>
+  <si>
+    <t>Abraham Arana</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>01:23:07</t>
+  </si>
+  <si>
+    <t>Mar 27 1:03PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Magallanes</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2017</t>
+  </si>
+  <si>
+    <t>01:52:21</t>
+  </si>
+  <si>
+    <t>Mar 27 7:22AM CST</t>
+  </si>
+  <si>
+    <t>Luis Ramirez</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>FORD F350 3MTS 2006</t>
+  </si>
+  <si>
+    <t>02:07:01</t>
+  </si>
+  <si>
+    <t>Mar 27 2:37PM CST</t>
+  </si>
+  <si>
+    <t>Alejandro Lara</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>WORKEN</t>
+  </si>
+  <si>
+    <t>00:18:15</t>
+  </si>
+  <si>
+    <t>Mar 27 3:10PM CST</t>
+  </si>
+  <si>
+    <t>Álvaro Zapata</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>KENWORTH</t>
+  </si>
+  <si>
+    <t>00:18:40</t>
+  </si>
+  <si>
+    <t>Mar 27 4:58PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Iñiguez</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>03:42:29</t>
+  </si>
+  <si>
+    <t>00:00:40</t>
+  </si>
+  <si>
+    <t>00:00:06</t>
+  </si>
+  <si>
+    <t>Mar 27 11:21AM CST</t>
+  </si>
+  <si>
+    <t>Mario Ballinas</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>01:12:21</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>00:00:35</t>
+  </si>
+  <si>
+    <t>Mar 27 12:07PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Ornelas</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2020</t>
+  </si>
+  <si>
+    <t>02:47:58</t>
+  </si>
+  <si>
+    <t>00:01:15</t>
+  </si>
+  <si>
+    <t>Mar 27 12:14PM CST</t>
+  </si>
+  <si>
+    <t>Moises Martinez</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>02:03:51</t>
+  </si>
+  <si>
+    <t>00:00:45</t>
+  </si>
+  <si>
+    <t>00:01:56</t>
+  </si>
+  <si>
+    <t>Mar 27 11:11AM CST</t>
+  </si>
+  <si>
+    <t>Eduardo Lopez</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>01:45:57</t>
+  </si>
+  <si>
+    <t>00:01:37</t>
+  </si>
+  <si>
+    <t>00:00:53</t>
+  </si>
+  <si>
+    <t>Adrian Caro</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>FORD RANGER 2011</t>
+  </si>
+  <si>
+    <t>03:10:41</t>
+  </si>
+  <si>
+    <t>00:02:20</t>
+  </si>
+  <si>
+    <t>00:01:51</t>
+  </si>
+  <si>
+    <t>Mar 27 4:25PM CST</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>02:17:54</t>
+  </si>
+  <si>
+    <t>00:02:21</t>
+  </si>
+  <si>
+    <t>00:02:17</t>
+  </si>
+  <si>
+    <t>Mar 27 12:15PM CST</t>
+  </si>
+  <si>
+    <t>Luis Galindo</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>KENWORTH 2009</t>
+  </si>
+  <si>
+    <t>07:49:35</t>
+  </si>
+  <si>
+    <t>00:06:48</t>
+  </si>
+  <si>
+    <t>00:10:33</t>
+  </si>
+  <si>
+    <t>00:01:17</t>
+  </si>
+  <si>
+    <t>Mar 27 6:50AM CST</t>
+  </si>
+  <si>
+    <t>Alberto Sanchez</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>VW DELIVERY 10.6</t>
+  </si>
+  <si>
+    <t>06:46:35</t>
+  </si>
+  <si>
+    <t>00:05:31</t>
+  </si>
+  <si>
+    <t>00:02:40</t>
+  </si>
+  <si>
+    <t>00:00:23</t>
+  </si>
+  <si>
+    <t>Alberto Jimenez</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>04:58:18</t>
+  </si>
+  <si>
+    <t>00:03:49</t>
+  </si>
+  <si>
+    <t>00:04:00</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>Mar 27 6:55PM CST</t>
+  </si>
+  <si>
+    <t>José Morales</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>02:42:53</t>
+  </si>
+  <si>
+    <t>00:01:06</t>
+  </si>
+  <si>
+    <t>00:00:58</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>00:00:12</t>
+  </si>
+  <si>
+    <t>Mar 27 1:33PM CST</t>
+  </si>
+  <si>
+    <t>Angel Cortez</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2018</t>
+  </si>
+  <si>
+    <t>03:39:20</t>
+  </si>
+  <si>
+    <t>00:01:40</t>
+  </si>
+  <si>
+    <t>00:01:04</t>
+  </si>
+  <si>
+    <t>Mar 27 10:33AM CST</t>
+  </si>
+  <si>
     <t>Diego Cardenas</t>
   </si>
   <si>
     <t>134</t>
   </si>
   <si>
-    <t>TOYOTA HILUX 2018</t>
-  </si>
-  <si>
-    <t>03:57:04</t>
-  </si>
-  <si>
-    <t>00:00:36</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
-    <t>Feb 12 1:58PM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Hernandez</t>
-  </si>
-  <si>
-    <t>152</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX</t>
-  </si>
-  <si>
-    <t>03:54:13</t>
+    <t>04:36:57</t>
+  </si>
+  <si>
+    <t>00:02:04</t>
+  </si>
+  <si>
+    <t>00:00:50</t>
   </si>
   <si>
     <t>00:00:04</t>
   </si>
   <si>
-    <t>Feb 12 3:57PM CST</t>
-  </si>
-  <si>
-    <t>Christian Aguilar</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2021</t>
-  </si>
-  <si>
-    <t>02:33:58</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>Feb 12 8:59AM CST</t>
-  </si>
-  <si>
-    <t>Hugo López</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>02:39:02</t>
-  </si>
-  <si>
-    <t>00:00:05</t>
-  </si>
-  <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>Feb 12 2:26PM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Lopez</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2020</t>
-  </si>
-  <si>
-    <t>01:48:08</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>Feb 12 2:03PM CST</t>
-  </si>
-  <si>
-    <t>Fernando Ornelas</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>01:47:37</t>
-  </si>
-  <si>
-    <t>Feb 12 1:34PM CST</t>
-  </si>
-  <si>
-    <t>Marcos Barbosa</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2023</t>
-  </si>
-  <si>
-    <t>02:23:33</t>
-  </si>
-  <si>
-    <t>Feb 12 1:49PM CST</t>
-  </si>
-  <si>
-    <t>Gerardo Aguillón</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>02:17:27</t>
-  </si>
-  <si>
-    <t>Feb 12 2:11PM CST</t>
-  </si>
-  <si>
-    <t>Abraham Arana</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>01:41:03</t>
-  </si>
-  <si>
-    <t>Feb 12 12:34PM CST</t>
+    <t>00:00:31</t>
+  </si>
+  <si>
+    <t>Mar 27 1:14PM CST</t>
   </si>
   <si>
     <t>Fernando Garcia</t>
@@ -267,49 +603,22 @@
     <t>Volkswagen</t>
   </si>
   <si>
-    <t>00:01:36</t>
-  </si>
-  <si>
-    <t>Feb 12 7:31AM CST</t>
-  </si>
-  <si>
-    <t>Luis Ramirez</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>FORD F350 3MTS 2006</t>
-  </si>
-  <si>
-    <t>03:03:30</t>
-  </si>
-  <si>
-    <t>00:00:41</t>
-  </si>
-  <si>
-    <t>00:01:32</t>
-  </si>
-  <si>
-    <t>Feb 12 12:01PM CST</t>
-  </si>
-  <si>
-    <t>José Morales</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>02:52:49</t>
-  </si>
-  <si>
-    <t>00:01:34</t>
-  </si>
-  <si>
-    <t>00:00:31</t>
-  </si>
-  <si>
-    <t>Feb 12 1:25PM CST</t>
+    <t>08:49:25</t>
+  </si>
+  <si>
+    <t>00:05:59</t>
+  </si>
+  <si>
+    <t>00:04:28</t>
+  </si>
+  <si>
+    <t>00:03:48</t>
+  </si>
+  <si>
+    <t>00:00:37</t>
+  </si>
+  <si>
+    <t>Mar 27 5:18PM CST</t>
   </si>
   <si>
     <t>Armando Muñoz</t>
@@ -321,91 +630,88 @@
     <t>HINO 300</t>
   </si>
   <si>
-    <t>02:28:29</t>
-  </si>
-  <si>
-    <t>00:00:55</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>Feb 12 3:17PM CST</t>
-  </si>
-  <si>
-    <t>Alejandro Lara</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>WORKEN</t>
-  </si>
-  <si>
-    <t>00:43:27</t>
-  </si>
-  <si>
-    <t>00:00:25</t>
-  </si>
-  <si>
-    <t>Feb 12 8:58AM CST</t>
-  </si>
-  <si>
-    <t>Mario Ballinas</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>03:59:57</t>
-  </si>
-  <si>
-    <t>00:02:14</t>
-  </si>
-  <si>
-    <t>00:03:08</t>
-  </si>
-  <si>
-    <t>Feb 12 4:24PM CST</t>
-  </si>
-  <si>
-    <t>Angel Cortez</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>04:11:32</t>
-  </si>
-  <si>
-    <t>00:02:40</t>
-  </si>
-  <si>
-    <t>00:01:02</t>
-  </si>
-  <si>
-    <t>00:00:09</t>
-  </si>
-  <si>
-    <t>Feb 12 1:12PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Sanchez</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>VW DELIVERY 10.6</t>
-  </si>
-  <si>
-    <t>01:26:07</t>
-  </si>
-  <si>
-    <t>00:02:22</t>
-  </si>
-  <si>
-    <t>Feb 12 10:46AM CST</t>
+    <t>05:16:21</t>
+  </si>
+  <si>
+    <t>00:05:04</t>
+  </si>
+  <si>
+    <t>00:06:01</t>
+  </si>
+  <si>
+    <t>00:02:02</t>
+  </si>
+  <si>
+    <t>Mar 27 10:22AM CST</t>
+  </si>
+  <si>
+    <t>Daniel Mercado</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>03:41:53</t>
+  </si>
+  <si>
+    <t>00:03:26</t>
+  </si>
+  <si>
+    <t>00:01:19</t>
+  </si>
+  <si>
+    <t>Mar 27 11:03AM CST</t>
+  </si>
+  <si>
+    <t>Emmanuel Salcedo</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>03:22:06</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>00:01:12</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
+  </si>
+  <si>
+    <t>00:00:32</t>
+  </si>
+  <si>
+    <t>David Serrano</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>02:36:18</t>
+  </si>
+  <si>
+    <t>00:02:11</t>
+  </si>
+  <si>
+    <t>00:02:05</t>
+  </si>
+  <si>
+    <t>Mar 27 11:22AM CST</t>
+  </si>
+  <si>
+    <t>Alberto Compras</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>NISSAN 1993</t>
+  </si>
+  <si>
+    <t>Sin ruta</t>
   </si>
   <si>
     <t>Jorge Tornero</t>
@@ -414,169 +720,13 @@
     <t>117</t>
   </si>
   <si>
-    <t>04:12:55</t>
-  </si>
-  <si>
-    <t>00:02:02</t>
-  </si>
-  <si>
-    <t>00:01:15</t>
-  </si>
-  <si>
-    <t>00:00:22</t>
-  </si>
-  <si>
-    <t>Feb 12 2:42PM CST</t>
-  </si>
-  <si>
-    <t>Luis Galindo</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>KENWORTH 2009</t>
-  </si>
-  <si>
-    <t>09:08:27</t>
-  </si>
-  <si>
-    <t>00:01:44</t>
-  </si>
-  <si>
-    <t>00:07:52</t>
-  </si>
-  <si>
-    <t>00:01:26</t>
-  </si>
-  <si>
-    <t>00:00:12</t>
-  </si>
-  <si>
-    <t>Feb 12 6:24AM CST</t>
-  </si>
-  <si>
-    <t>Luis Ibarra</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2024</t>
-  </si>
-  <si>
-    <t>04:42:16</t>
-  </si>
-  <si>
-    <t>00:00:44</t>
-  </si>
-  <si>
-    <t>00:00:53</t>
-  </si>
-  <si>
-    <t>00:00:28</t>
-  </si>
-  <si>
-    <t>Feb 12 1:47PM CST</t>
-  </si>
-  <si>
-    <t>Miguel Guizar</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Hino 300 2024</t>
-  </si>
-  <si>
-    <t>08:56:41</t>
-  </si>
-  <si>
-    <t>00:05:09</t>
-  </si>
-  <si>
-    <t>00:03:14</t>
-  </si>
-  <si>
-    <t>00:02:29</t>
-  </si>
-  <si>
-    <t>00:00:29</t>
-  </si>
-  <si>
-    <t>Feb 12 2:48PM CST</t>
-  </si>
-  <si>
-    <t>Daniel Iñiguez</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2017</t>
-  </si>
-  <si>
-    <t>04:11:04</t>
-  </si>
-  <si>
-    <t>00:01:38</t>
-  </si>
-  <si>
-    <t>00:01:51</t>
-  </si>
-  <si>
-    <t>00:00:23</t>
-  </si>
-  <si>
-    <t>Feb 12 1:04PM CST</t>
-  </si>
-  <si>
-    <t>Francisco Marquez</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-  </si>
-  <si>
-    <t>08:41:12</t>
-  </si>
-  <si>
-    <t>00:18:07</t>
-  </si>
-  <si>
-    <t>00:06:34</t>
-  </si>
-  <si>
-    <t>00:04:08</t>
-  </si>
-  <si>
-    <t>00:00:47</t>
-  </si>
-  <si>
-    <t>Feb 12 10:53AM CST</t>
-  </si>
-  <si>
-    <t>Daniel Mercado</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>03:22:57</t>
-  </si>
-  <si>
-    <t>00:03:45</t>
-  </si>
-  <si>
-    <t>00:01:20</t>
-  </si>
-  <si>
-    <t>00:00:40</t>
-  </si>
-  <si>
-    <t>Feb 12 1:28PM CST</t>
+    <t>Martin Quezada</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>INTERNACIONAL</t>
   </si>
   <si>
     <t>Miguel Zamora</t>
@@ -585,178 +735,19 @@
     <t>139</t>
   </si>
   <si>
-    <t>14:23:16</t>
-  </si>
-  <si>
-    <t>00:11:12</t>
-  </si>
-  <si>
-    <t>00:14:23</t>
-  </si>
-  <si>
-    <t>00:10:53</t>
-  </si>
-  <si>
-    <t>00:04:32</t>
-  </si>
-  <si>
-    <t>Feb 12 7:51PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Jimenez</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>VAN HYUNDAI</t>
-  </si>
-  <si>
-    <t>04:38:01</t>
-  </si>
-  <si>
-    <t>00:02:58</t>
-  </si>
-  <si>
-    <t>00:01:57</t>
-  </si>
-  <si>
-    <t>00:02:01</t>
-  </si>
-  <si>
-    <t>Feb 12 5:42PM CST</t>
+    <t>Alexis Alvarado</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>HINO 500</t>
   </si>
   <si>
     <t>Alejandro Suarez</t>
   </si>
   <si>
     <t>146</t>
-  </si>
-  <si>
-    <t>HINO 500</t>
-  </si>
-  <si>
-    <t>07:01:53</t>
-  </si>
-  <si>
-    <t>00:06:00</t>
-  </si>
-  <si>
-    <t>00:05:50</t>
-  </si>
-  <si>
-    <t>00:05:19</t>
-  </si>
-  <si>
-    <t>00:09:12</t>
-  </si>
-  <si>
-    <t>Feb 12 4:12PM CST</t>
-  </si>
-  <si>
-    <t>Martin Quezada</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>INTERNACIONAL</t>
-  </si>
-  <si>
-    <t>06:19:36</t>
-  </si>
-  <si>
-    <t>00:03:35</t>
-  </si>
-  <si>
-    <t>00:05:46</t>
-  </si>
-  <si>
-    <t>00:00:37</t>
-  </si>
-  <si>
-    <t>Feb 12 1:19PM CST</t>
-  </si>
-  <si>
-    <t>Emmanuel Salcedo</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>03:26:19</t>
-  </si>
-  <si>
-    <t>00:01:05</t>
-  </si>
-  <si>
-    <t>00:01:22</t>
-  </si>
-  <si>
-    <t>Feb 12 4:37PM CST</t>
-  </si>
-  <si>
-    <t>Moises Martinez</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>03:12:14</t>
-  </si>
-  <si>
-    <t>00:01:18</t>
-  </si>
-  <si>
-    <t>00:01:23</t>
-  </si>
-  <si>
-    <t>Feb 12 9:46AM CST</t>
-  </si>
-  <si>
-    <t>Alberto Compras</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>NISSAN 1993</t>
-  </si>
-  <si>
-    <t>Sin ruta</t>
-  </si>
-  <si>
-    <t>Kevin De La O</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>Adrian Caro</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>FORD RANGER 2011</t>
-  </si>
-  <si>
-    <t>Álvaro Zapata</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>KENWORTH</t>
-  </si>
-  <si>
-    <t>Alexis Alvarado</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
 </sst>
 </file>
@@ -864,8 +855,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AE36">
-  <autoFilter ref="A1:AE36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AE39">
+  <autoFilter ref="A1:AE39"/>
   <tableColumns count="31">
     <tableColumn id="1" name="Operador"/>
     <tableColumn id="2" name="Número de unidad"/>
@@ -1188,11 +1179,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G18" sqref="G18"/>
+      <selection pane="topRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,10 +1332,10 @@
         <v>34</v>
       </c>
       <c r="F2" s="1">
-        <v>79.900000000000006</v>
+        <v>139.1</v>
       </c>
       <c r="G2" s="1">
-        <v>11.73</v>
+        <v>12.89</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1356,10 +1347,10 @@
         <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -1374,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>81.010000000000005</v>
+        <v>94.01</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -1398,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z2" s="1">
         <v>0</v>
@@ -1421,40 +1412,40 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1">
-        <v>59.1</v>
+        <v>54</v>
       </c>
       <c r="G3" s="1">
-        <v>8.52</v>
+        <v>7.77</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -1469,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S3" s="1">
         <v>0</v>
@@ -1493,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z3" s="1">
         <v>0</v>
@@ -1516,40 +1507,40 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1">
-        <v>38.200000000000003</v>
+        <v>48.2</v>
       </c>
       <c r="G4" s="1">
-        <v>6.19</v>
+        <v>5.85</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
@@ -1588,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z4" s="1">
         <v>0</v>
@@ -1617,53 +1608,53 @@
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1">
-        <v>35.4</v>
-      </c>
-      <c r="G5" s="1">
-        <v>7.06</v>
+        <v>44.8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>81.040000000000006</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>60</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
@@ -1683,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z5" s="1">
         <v>0</v>
@@ -1706,59 +1697,59 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="1">
+        <v>41.8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="1">
-        <v>29.3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5.61</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>71.010000000000005</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="S6" s="1">
         <v>0</v>
       </c>
@@ -1778,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z6" s="1">
         <v>0</v>
@@ -1801,13 +1792,13 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D7" s="2">
         <v>100</v>
@@ -1816,25 +1807,25 @@
         <v>64</v>
       </c>
       <c r="F7" s="1">
-        <v>29.1</v>
+        <v>38.9</v>
       </c>
       <c r="G7" s="1">
-        <v>4.87</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
@@ -1849,10 +1840,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1">
-        <v>59</v>
+        <v>76.010000000000005</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S7" s="1">
         <v>0</v>
@@ -1873,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z7" s="1">
         <v>0</v>
@@ -1896,13 +1887,13 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
@@ -1911,25 +1902,25 @@
         <v>69</v>
       </c>
       <c r="F8" s="1">
-        <v>27.7</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="G8" s="1">
-        <v>4.3099999999999996</v>
+        <v>6.03</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -1944,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>70</v>
@@ -1968,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z8" s="1">
         <v>0</v>
@@ -1997,34 +1988,34 @@
         <v>72</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2">
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1">
-        <v>26.7</v>
+        <v>30.1</v>
       </c>
       <c r="G9" s="1">
-        <v>4.7699999999999996</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -2042,7 +2033,7 @@
         <v>50</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -2063,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z9" s="1">
         <v>0</v>
@@ -2086,40 +2077,40 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
         <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1">
-        <v>19.600000000000001</v>
+        <v>28.9</v>
       </c>
       <c r="G10" s="1">
-        <v>4.03</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -2134,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -2158,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z10" s="1">
         <v>0</v>
@@ -2181,13 +2172,13 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2">
         <v>100</v>
@@ -2196,25 +2187,25 @@
         <v>82</v>
       </c>
       <c r="F11" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>245</v>
+        <v>24.3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3.2</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -2229,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1">
-        <v>23.49</v>
+        <v>62</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>83</v>
@@ -2253,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z11" s="1">
         <v>0</v>
@@ -2285,50 +2276,50 @@
         <v>86</v>
       </c>
       <c r="D12" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F12" s="1">
-        <v>62.9</v>
+        <v>24.3</v>
       </c>
       <c r="G12" s="1">
-        <v>16.02</v>
+        <v>2.27</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>52</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>76.010000000000005</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="S12" s="1">
         <v>0</v>
       </c>
@@ -2348,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z12" s="1">
         <v>0</v>
@@ -2371,59 +2362,59 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="2">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2">
-        <v>99</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1">
+        <v>21.1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>9.86</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>50</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="1">
-        <v>55.2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>7.95</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>73.010000000000005</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="S13" s="1">
         <v>0</v>
       </c>
@@ -2443,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z13" s="1">
         <v>0</v>
@@ -2466,59 +2457,59 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>36</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="2">
-        <v>99</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="1">
-        <v>46.7</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6.51</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>72.010000000000005</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="S14" s="1">
         <v>0</v>
       </c>
@@ -2538,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z14" s="1">
         <v>0</v>
@@ -2561,40 +2552,40 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D15" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F15" s="1">
-        <v>19.399999999999999</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G15" s="1">
-        <v>6</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
@@ -2609,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2633,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z15" s="1">
         <v>0</v>
@@ -2656,40 +2647,40 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F16" s="1">
-        <v>78.2</v>
+        <v>69.7</v>
       </c>
       <c r="G16" s="1">
-        <v>12.32</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
@@ -2704,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1">
-        <v>91.01</v>
+        <v>71.010000000000005</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
@@ -2728,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
@@ -2751,40 +2742,40 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F17" s="1">
-        <v>110</v>
+        <v>26.8</v>
       </c>
       <c r="G17" s="1">
-        <v>14.83</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
@@ -2799,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>77.010000000000005</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="S17" s="1">
         <v>0</v>
@@ -2823,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
@@ -2846,40 +2837,40 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F18" s="1">
-        <v>47.8</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>245</v>
+        <v>61.1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>7.69</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
@@ -2894,10 +2885,10 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1">
-        <v>93.89</v>
+        <v>80.010000000000005</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="S18" s="1">
         <v>0</v>
@@ -2918,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
@@ -2941,40 +2932,40 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F19" s="1">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="G19" s="1">
-        <v>8.34</v>
+        <v>6.63</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>134</v>
+        <v>37</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="M19" s="1">
         <v>0</v>
@@ -2989,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1">
-        <v>71.010000000000005</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -3013,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
@@ -3036,46 +3027,46 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F20" s="1">
-        <v>557</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="G20" s="1">
-        <v>134.88</v>
+        <v>6.57</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>142</v>
+        <v>59</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>143</v>
+        <v>37</v>
       </c>
       <c r="M20" s="1">
         <v>0</v>
       </c>
       <c r="N20" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O20" s="1">
         <v>0</v>
@@ -3084,10 +3075,10 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1">
-        <v>97.01</v>
+        <v>70.010000000000005</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="S20" s="1">
         <v>0</v>
@@ -3108,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
@@ -3131,40 +3122,40 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="F21" s="1">
-        <v>121.9</v>
+        <v>59.5</v>
       </c>
       <c r="G21" s="1">
-        <v>17.54</v>
+        <v>8.08</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>151</v>
+        <v>65</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="M21" s="1">
         <v>0</v>
@@ -3179,10 +3170,10 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1">
-        <v>87.01</v>
+        <v>88.01</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -3203,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
@@ -3226,40 +3217,40 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="3">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="D22" s="2">
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F22" s="1">
-        <v>500.6</v>
+        <v>48.3</v>
       </c>
       <c r="G22" s="1">
-        <v>70.099999999999994</v>
+        <v>3.97</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>159</v>
+        <v>65</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
@@ -3274,10 +3265,10 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1">
-        <v>111.01</v>
+        <v>90.01</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="S22" s="1">
         <v>0</v>
@@ -3298,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z22" s="1">
         <v>0</v>
@@ -3321,46 +3312,46 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="D23" s="3">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="F23" s="1">
-        <v>78.900000000000006</v>
+        <v>400.9</v>
       </c>
       <c r="G23" s="1">
-        <v>10.06</v>
+        <v>95.15</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
       <c r="M23" s="1">
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O23" s="1">
         <v>0</v>
@@ -3369,10 +3360,10 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>71.010000000000005</v>
+        <v>97.01</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="S23" s="1">
         <v>0</v>
@@ -3393,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z23" s="1">
         <v>0</v>
@@ -3416,40 +3407,40 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" s="4">
-        <v>66</v>
+        <v>156</v>
+      </c>
+      <c r="D24" s="3">
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F24" s="1">
-        <v>620.6</v>
-      </c>
-      <c r="G24" s="1">
-        <v>165.99</v>
+        <v>324.5</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>177</v>
+        <v>36</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
@@ -3464,10 +3455,10 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>97.01</v>
+        <v>96.91</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>178</v>
+        <v>98</v>
       </c>
       <c r="S24" s="1">
         <v>0</v>
@@ -3488,7 +3479,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
@@ -3511,46 +3502,46 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="3">
+        <v>85</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="1">
+        <v>97</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="4">
-        <v>52</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F25" s="1">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="G25" s="1">
-        <v>11.15</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="J25" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -3559,10 +3550,10 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1">
-        <v>85.01</v>
+        <v>101.42</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="S25" s="1">
         <v>0</v>
@@ -3583,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z25" s="1">
         <v>0</v>
@@ -3606,40 +3597,40 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="4">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="3">
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="F26" s="1">
-        <v>717.1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>245</v>
+        <v>45.3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>6.94</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="M26" s="1">
         <v>0</v>
@@ -3648,16 +3639,16 @@
         <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="1">
-        <v>102.96</v>
+        <v>71.010000000000005</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="S26" s="1">
         <v>0</v>
@@ -3678,7 +3669,7 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z26" s="1">
         <v>0</v>
@@ -3701,40 +3692,40 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D27" s="4">
-        <v>13</v>
+        <v>178</v>
+      </c>
+      <c r="D27" s="3">
+        <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="F27" s="1">
-        <v>139.80000000000001</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>245</v>
+        <v>112.2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>14.75</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>200</v>
+        <v>65</v>
       </c>
       <c r="M27" s="1">
         <v>0</v>
@@ -3749,10 +3740,10 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1">
-        <v>125.73</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
@@ -3773,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -3796,40 +3787,40 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
+        <v>178</v>
+      </c>
+      <c r="D28" s="3">
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="F28" s="1">
-        <v>363.1</v>
+        <v>101.4</v>
       </c>
       <c r="G28" s="1">
-        <v>84.38</v>
+        <v>13.7</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
@@ -3841,13 +3832,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="1">
-        <v>109.01</v>
+        <v>84.01</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -3868,7 +3859,7 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z28" s="1">
         <v>0</v>
@@ -3891,64 +3882,64 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
+        <v>193</v>
+      </c>
+      <c r="D29" s="3">
+        <v>73</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="F29" s="1">
-        <v>321.39999999999998</v>
-      </c>
-      <c r="G29" s="1">
-        <v>110.96</v>
+        <v>427.7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
         <v>1</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="M29" s="1">
-        <v>0</v>
-      </c>
-      <c r="N29" s="1">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1">
-        <v>2</v>
-      </c>
       <c r="P29" s="1">
         <v>0</v>
       </c>
       <c r="Q29" s="1">
-        <v>100.01</v>
+        <v>96.97</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="S29" s="1">
         <v>0</v>
       </c>
       <c r="T29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U29" s="1">
         <v>0</v>
@@ -3963,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z29" s="1">
         <v>0</v>
@@ -3986,46 +3977,46 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="F30" s="1">
-        <v>60.7</v>
+        <v>238.8</v>
       </c>
       <c r="G30" s="1">
-        <v>13</v>
+        <v>32.06</v>
       </c>
       <c r="H30" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="M30" s="1">
         <v>0</v>
       </c>
       <c r="N30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="1">
         <v>0</v>
@@ -4034,10 +4025,10 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1">
-        <v>72.010000000000005</v>
+        <v>90.01</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="S30" s="1">
         <v>0</v>
@@ -4049,7 +4040,7 @@
         <v>0</v>
       </c>
       <c r="V30" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W30" s="1">
         <v>0</v>
@@ -4058,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z30" s="1">
         <v>0</v>
@@ -4070,7 +4061,7 @@
         <v>0</v>
       </c>
       <c r="AC30" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD30" s="1">
         <v>0</v>
@@ -4081,40 +4072,40 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="D31" s="4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F31" s="1">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G31" s="1">
-        <v>10.61</v>
+        <v>11.34</v>
       </c>
       <c r="H31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>228</v>
+        <v>166</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>36</v>
+        <v>212</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
@@ -4129,16 +4120,16 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1">
-        <v>78.010000000000005</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="S31" s="1">
         <v>0</v>
       </c>
       <c r="T31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31" s="1">
         <v>0</v>
@@ -4153,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z31" s="1">
         <v>0</v>
@@ -4176,477 +4167,762 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="S32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="T32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="U32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="V32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Y32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AB32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AD32" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AE32" s="6" t="s">
-        <v>234</v>
+        <v>86</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" s="1">
+        <v>59.4</v>
+      </c>
+      <c r="G32" s="1">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>88.01</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0</v>
+      </c>
+      <c r="U32" s="1">
+        <v>0</v>
+      </c>
+      <c r="V32" s="1">
+        <v>1</v>
+      </c>
+      <c r="W32" s="1">
+        <v>0</v>
+      </c>
+      <c r="X32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="T33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="U33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="V33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="X33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Y33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AA33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AB33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AD33" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="AE33" s="6" t="s">
-        <v>234</v>
+        <v>86</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" s="1">
+        <v>53.1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4.71</v>
+      </c>
+      <c r="H33" s="1">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>84.01</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>2</v>
+      </c>
+      <c r="U33" s="1">
+        <v>1</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0</v>
+      </c>
+      <c r="X33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="R34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="U34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="W34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="X34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Y34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Z34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AA34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AB34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AC34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AD34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AE34" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Q35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="R35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="U35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="X35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Y35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Z35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AA35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AB35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AC35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AD35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AE35" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="X36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Y36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Z36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AA36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AB36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AC36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AD36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AE36" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="T37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="U37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="V37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="W37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="X37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD37" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE37" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="X38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD38" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE38" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="W39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="X39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD39" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE39" s="6" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de archivos en la carpeta data - 2025-05-20 11:08:46
</commit_message>
<xml_diff>
--- a/data/Informe_Diario_Unidades.xlsx
+++ b/data/Informe_Diario_Unidades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="257">
   <si>
     <t>Operador</t>
   </si>
@@ -117,6 +117,198 @@
     <t>Comer/Beber (Manual)</t>
   </si>
   <si>
+    <t>José Morales</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2021</t>
+  </si>
+  <si>
+    <t>03:19:48</t>
+  </si>
+  <si>
+    <t>00:00:45</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>May 15 3:10PM CST</t>
+  </si>
+  <si>
+    <t>Sin ruta.</t>
+  </si>
+  <si>
+    <t>Alejandro Lara</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>WORKEN</t>
+  </si>
+  <si>
+    <t>02:10:37</t>
+  </si>
+  <si>
+    <t>May 15 11:06AM CST</t>
+  </si>
+  <si>
+    <t>Christian Aguilar</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>03:20:40</t>
+  </si>
+  <si>
+    <t>May 15 1:47PM CST</t>
+  </si>
+  <si>
+    <t>Gerardo Aguillón</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>03:16:03</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>May 15 2:11PM CST</t>
+  </si>
+  <si>
+    <t>Hugo López</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX</t>
+  </si>
+  <si>
+    <t>02:20:47</t>
+  </si>
+  <si>
+    <t>May 15 11:24AM CST</t>
+  </si>
+  <si>
+    <t>Marcos Barbosa</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2023</t>
+  </si>
+  <si>
+    <t>02:18:46</t>
+  </si>
+  <si>
+    <t>May 15 8:24AM CST</t>
+  </si>
+  <si>
+    <t>Luis Ramirez</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>FORD F350 3MTS 2006</t>
+  </si>
+  <si>
+    <t>02:03:36</t>
+  </si>
+  <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
+    <t>May 15 12:28PM CST</t>
+  </si>
+  <si>
+    <t>Álvaro Zapata</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>KENWORTH</t>
+  </si>
+  <si>
+    <t>00:47:51</t>
+  </si>
+  <si>
+    <t>May 15 4:45PM CST</t>
+  </si>
+  <si>
+    <t>Alexis Alvarado</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>HINO 500</t>
+  </si>
+  <si>
+    <t>00:01:19</t>
+  </si>
+  <si>
+    <t>May 15 6:33PM CST</t>
+  </si>
+  <si>
+    <t>Francisco Marquez</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+  </si>
+  <si>
+    <t>00:01:28</t>
+  </si>
+  <si>
+    <t>May 15 6:27PM CST</t>
+  </si>
+  <si>
+    <t>Adrian Caro</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>FORD RANGER 2011</t>
+  </si>
+  <si>
+    <t>00:01:26</t>
+  </si>
+  <si>
+    <t>May 15 2:51PM CST</t>
+  </si>
+  <si>
+    <t>Miguel Guizar</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Hino 300 2024</t>
+  </si>
+  <si>
+    <t>00:00:46</t>
+  </si>
+  <si>
+    <t>May 15 11:05AM CST</t>
+  </si>
+  <si>
     <t>Luis Ibarra</t>
   </si>
   <si>
@@ -126,19 +318,379 @@
     <t>TOYOTA HILUX 2024</t>
   </si>
   <si>
-    <t>03:22:16</t>
-  </si>
-  <si>
-    <t>00:00:27</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
-  </si>
-  <si>
-    <t>Apr 3 11:06AM CST</t>
-  </si>
-  <si>
-    <t>Sin ruta.</t>
+    <t>04:47:30</t>
+  </si>
+  <si>
+    <t>00:01:38</t>
+  </si>
+  <si>
+    <t>May 15 1:15PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Magallanes</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2017</t>
+  </si>
+  <si>
+    <t>02:58:50</t>
+  </si>
+  <si>
+    <t>00:01:23</t>
+  </si>
+  <si>
+    <t>00:00:37</t>
+  </si>
+  <si>
+    <t>May 15 11:46AM CST</t>
+  </si>
+  <si>
+    <t>Angel Cortez</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2018</t>
+  </si>
+  <si>
+    <t>04:35:37</t>
+  </si>
+  <si>
+    <t>00:03:18</t>
+  </si>
+  <si>
+    <t>00:01:17</t>
+  </si>
+  <si>
+    <t>May 15 3:22PM CST</t>
+  </si>
+  <si>
+    <t>Daniel Iñiguez</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>03:40:26</t>
+  </si>
+  <si>
+    <t>00:01:24</t>
+  </si>
+  <si>
+    <t>00:00:57</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
+  </si>
+  <si>
+    <t>May 15 9:32AM CST</t>
+  </si>
+  <si>
+    <t>Fernando Ornelas</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>TOYOTA HILUX 2020</t>
+  </si>
+  <si>
+    <t>02:44:07</t>
+  </si>
+  <si>
+    <t>00:01:14</t>
+  </si>
+  <si>
+    <t>00:01:58</t>
+  </si>
+  <si>
+    <t>May 15 11:40AM CST</t>
+  </si>
+  <si>
+    <t>Moises Martinez</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>02:00:53</t>
+  </si>
+  <si>
+    <t>00:00:33</t>
+  </si>
+  <si>
+    <t>00:00:54</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>May 15 1:42PM CST</t>
+  </si>
+  <si>
+    <t>Emmanuel Salcedo</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>03:25:38</t>
+  </si>
+  <si>
+    <t>00:02:36</t>
+  </si>
+  <si>
+    <t>00:01:55</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
+  </si>
+  <si>
+    <t>Kevin De La O</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>VAN HYUNDAI</t>
+  </si>
+  <si>
+    <t>03:42:54</t>
+  </si>
+  <si>
+    <t>00:03:33</t>
+  </si>
+  <si>
+    <t>00:02:42</t>
+  </si>
+  <si>
+    <t>May 15 2:58PM CST</t>
+  </si>
+  <si>
+    <t>Armando Muñoz</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>HINO 300</t>
+  </si>
+  <si>
+    <t>04:07:23</t>
+  </si>
+  <si>
+    <t>00:02:10</t>
+  </si>
+  <si>
+    <t>00:00:21</t>
+  </si>
+  <si>
+    <t>00:00:50</t>
+  </si>
+  <si>
+    <t>May 15 3:16PM CST</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>01:46:08</t>
+  </si>
+  <si>
+    <t>00:02:54</t>
+  </si>
+  <si>
+    <t>00:01:45</t>
+  </si>
+  <si>
+    <t>May 15 9:30AM CST</t>
+  </si>
+  <si>
+    <t>Jorge Tornero</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>02:59:25</t>
+  </si>
+  <si>
+    <t>00:00:52</t>
+  </si>
+  <si>
+    <t>00:00:12</t>
+  </si>
+  <si>
+    <t>May 15 9:18AM CST</t>
+  </si>
+  <si>
+    <t>Alberto Jimenez</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>03:33:37</t>
+  </si>
+  <si>
+    <t>00:02:45</t>
+  </si>
+  <si>
+    <t>00:02:48</t>
+  </si>
+  <si>
+    <t>May 15 4:24PM CST</t>
+  </si>
+  <si>
+    <t>Alberto Sanchez</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>VW DELIVERY 10.6</t>
+  </si>
+  <si>
+    <t>06:16:30</t>
+  </si>
+  <si>
+    <t>00:08:46</t>
+  </si>
+  <si>
+    <t>00:05:28</t>
+  </si>
+  <si>
+    <t>00:01:13</t>
+  </si>
+  <si>
+    <t>00:00:32</t>
+  </si>
+  <si>
+    <t>May 15 2:23PM CST</t>
+  </si>
+  <si>
+    <t>Fernando Garcia</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>08:59:50</t>
+  </si>
+  <si>
+    <t>00:06:27</t>
+  </si>
+  <si>
+    <t>00:05:14</t>
+  </si>
+  <si>
+    <t>00:05:31</t>
+  </si>
+  <si>
+    <t>00:00:42</t>
+  </si>
+  <si>
+    <t>May 15 5:08PM CST</t>
+  </si>
+  <si>
+    <t>Luis Galindo</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>KENWORTH 2009</t>
+  </si>
+  <si>
+    <t>06:55:25</t>
+  </si>
+  <si>
+    <t>00:08:17</t>
+  </si>
+  <si>
+    <t>00:12:20</t>
+  </si>
+  <si>
+    <t>00:04:39</t>
+  </si>
+  <si>
+    <t>00:01:20</t>
+  </si>
+  <si>
+    <t>May 15 6:35AM CST</t>
+  </si>
+  <si>
+    <t>Daniel Mercado</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>04:59:36</t>
+  </si>
+  <si>
+    <t>00:04:17</t>
+  </si>
+  <si>
+    <t>00:02:11</t>
+  </si>
+  <si>
+    <t>May 15 4:05PM CST</t>
+  </si>
+  <si>
+    <t>Mario Ballinas</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>04:18:18</t>
+  </si>
+  <si>
+    <t>00:06:22</t>
+  </si>
+  <si>
+    <t>00:09:47</t>
+  </si>
+  <si>
+    <t>00:02:00</t>
+  </si>
+  <si>
+    <t>00:01:31</t>
+  </si>
+  <si>
+    <t>May 15 4:04PM CST</t>
+  </si>
+  <si>
+    <t>Diego Cardenas</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>05:07:10</t>
+  </si>
+  <si>
+    <t>00:01:07</t>
+  </si>
+  <si>
+    <t>00:00:43</t>
+  </si>
+  <si>
+    <t>00:00:39</t>
+  </si>
+  <si>
+    <t>May 15 10:56AM CST</t>
   </si>
   <si>
     <t>Eduardo Hernandez</t>
@@ -147,238 +699,31 @@
     <t>152</t>
   </si>
   <si>
-    <t>TOYOTA HILUX</t>
-  </si>
-  <si>
-    <t>03:16:41</t>
-  </si>
-  <si>
-    <t>00:00:23</t>
-  </si>
-  <si>
-    <t>Apr 3 2:15PM CST</t>
-  </si>
-  <si>
-    <t>Christian Aguilar</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2021</t>
-  </si>
-  <si>
-    <t>03:25:38</t>
-  </si>
-  <si>
-    <t>00:00:22</t>
-  </si>
-  <si>
-    <t>Apr 3 12:28PM CST</t>
-  </si>
-  <si>
-    <t>Gerardo Aguillón</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>02:16:48</t>
-  </si>
-  <si>
-    <t>Apr 3 8:23AM CST</t>
-  </si>
-  <si>
-    <t>Hugo López</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>01:51:38</t>
-  </si>
-  <si>
-    <t>Apr 3 1:58PM CST</t>
-  </si>
-  <si>
-    <t>Marcos Barbosa</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2023</t>
-  </si>
-  <si>
-    <t>02:19:54</t>
-  </si>
-  <si>
-    <t>00:00:05</t>
-  </si>
-  <si>
-    <t>Apr 3 2:10PM CST</t>
-  </si>
-  <si>
-    <t>Mario Ballinas</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>01:31:59</t>
-  </si>
-  <si>
-    <t>Apr 3 8:26AM CST</t>
-  </si>
-  <si>
-    <t>Daniel Magallanes</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2017</t>
-  </si>
-  <si>
-    <t>01:09:56</t>
-  </si>
-  <si>
-    <t>Apr 3 7:38AM CST</t>
-  </si>
-  <si>
-    <t>Luis Ramirez</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>FORD F350 3MTS 2006</t>
-  </si>
-  <si>
-    <t>00:13:55</t>
-  </si>
-  <si>
-    <t>Apr 3 5:49PM CST</t>
-  </si>
-  <si>
-    <t>Álvaro Zapata</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>KENWORTH</t>
-  </si>
-  <si>
-    <t>00:18:56</t>
-  </si>
-  <si>
-    <t>Apr 3 4:26PM CST</t>
-  </si>
-  <si>
-    <t>Alejandro Lara</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>WORKEN</t>
-  </si>
-  <si>
-    <t>00:16:06</t>
-  </si>
-  <si>
-    <t>Apr 3 4:24PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Sanchez</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>VW DELIVERY 10.6</t>
-  </si>
-  <si>
-    <t>00:16:12</t>
-  </si>
-  <si>
-    <t>Apr 3 4:46PM CST</t>
-  </si>
-  <si>
-    <t>Francisco Marquez</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-  </si>
-  <si>
-    <t>00:01:37</t>
-  </si>
-  <si>
-    <t>Apr 3 7:50PM CST</t>
-  </si>
-  <si>
-    <t>Miguel Guizar</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Hino 300 2024</t>
-  </si>
-  <si>
-    <t>05:19:12</t>
-  </si>
-  <si>
-    <t>00:02:55</t>
-  </si>
-  <si>
-    <t>00:00:39</t>
-  </si>
-  <si>
-    <t>Apr 3 5:52PM CST</t>
-  </si>
-  <si>
-    <t>José Morales</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>02:51:25</t>
-  </si>
-  <si>
-    <t>00:01:22</t>
-  </si>
-  <si>
-    <t>00:00:06</t>
-  </si>
-  <si>
-    <t>Apr 3 1:21PM CST</t>
-  </si>
-  <si>
-    <t>Adrian Caro</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>FORD RANGER 2011</t>
-  </si>
-  <si>
-    <t>02:55:26</t>
-  </si>
-  <si>
-    <t>00:00:42</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>Apr 3 7:37PM CST</t>
+    <t>03:22:29</t>
+  </si>
+  <si>
+    <t>00:01:04</t>
+  </si>
+  <si>
+    <t>May 15 2:55PM CST</t>
+  </si>
+  <si>
+    <t>Eduardo Lopez</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>02:31:40</t>
+  </si>
+  <si>
+    <t>00:00:40</t>
+  </si>
+  <si>
+    <t>00:00:15</t>
+  </si>
+  <si>
+    <t>May 15 4:19PM CST</t>
   </si>
   <si>
     <t>Abraham Arana</t>
@@ -387,391 +732,64 @@
     <t>140</t>
   </si>
   <si>
-    <t>02:17:30</t>
-  </si>
-  <si>
-    <t>00:01:14</t>
-  </si>
-  <si>
-    <t>00:00:48</t>
-  </si>
-  <si>
-    <t>Apr 3 12:44PM CST</t>
-  </si>
-  <si>
-    <t>Daniel Iñiguez</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>03:57:17</t>
-  </si>
-  <si>
-    <t>00:01:07</t>
-  </si>
-  <si>
-    <t>00:00:33</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>Apr 3 10:26AM CST</t>
-  </si>
-  <si>
-    <t>Eduardo Lopez</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2020</t>
-  </si>
-  <si>
-    <t>03:21:28</t>
-  </si>
-  <si>
-    <t>00:01:12</t>
-  </si>
-  <si>
-    <t>00:01:10</t>
+    <t>02:14:09</t>
+  </si>
+  <si>
+    <t>00:01:15</t>
+  </si>
+  <si>
+    <t>May 15 10:36AM CST</t>
+  </si>
+  <si>
+    <t>David Serrano</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>01:50:30</t>
+  </si>
+  <si>
+    <t>00:02:32</t>
+  </si>
+  <si>
+    <t>00:00:16</t>
+  </si>
+  <si>
+    <t>May 15 11:54AM CST</t>
+  </si>
+  <si>
+    <t>Alberto Compras</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>NISSAN 1993</t>
+  </si>
+  <si>
+    <t>Sin ruta</t>
+  </si>
+  <si>
+    <t>Martin Quezada</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>Miguel Zamora</t>
+  </si>
+  <si>
+    <t>139</t>
   </si>
   <si>
     <t>Alejandro Suarez</t>
   </si>
   <si>
     <t>146</t>
-  </si>
-  <si>
-    <t>HINO 500</t>
-  </si>
-  <si>
-    <t>02:42:05</t>
-  </si>
-  <si>
-    <t>00:01:18</t>
-  </si>
-  <si>
-    <t>00:00:38</t>
-  </si>
-  <si>
-    <t>Apr 3 10:22AM CST</t>
-  </si>
-  <si>
-    <t>Moises Martinez</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>02:29:24</t>
-  </si>
-  <si>
-    <t>00:00:58</t>
-  </si>
-  <si>
-    <t>00:00:32</t>
-  </si>
-  <si>
-    <t>Apr 3 2:38PM CST</t>
-  </si>
-  <si>
-    <t>Angel Cortez</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>TOYOTA HILUX 2018</t>
-  </si>
-  <si>
-    <t>05:28:46</t>
-  </si>
-  <si>
-    <t>00:03:45</t>
-  </si>
-  <si>
-    <t>00:05:16</t>
-  </si>
-  <si>
-    <t>00:00:16</t>
-  </si>
-  <si>
-    <t>Apr 3 12:41PM CST</t>
-  </si>
-  <si>
-    <t>Diego Cardenas</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>05:49:19</t>
-  </si>
-  <si>
-    <t>00:02:21</t>
-  </si>
-  <si>
-    <t>00:02:26</t>
-  </si>
-  <si>
-    <t>Apr 3 1:49PM CST</t>
-  </si>
-  <si>
-    <t>Luis Galindo</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>KENWORTH 2009</t>
-  </si>
-  <si>
-    <t>06:43:42</t>
-  </si>
-  <si>
-    <t>00:05:40</t>
-  </si>
-  <si>
-    <t>00:14:05</t>
-  </si>
-  <si>
-    <t>00:02:33</t>
-  </si>
-  <si>
-    <t>Apr 3 3:28PM CST</t>
-  </si>
-  <si>
-    <t>Kevin De La O</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>VAN HYUNDAI</t>
-  </si>
-  <si>
-    <t>02:48:30</t>
-  </si>
-  <si>
-    <t>00:04:03</t>
-  </si>
-  <si>
-    <t>00:02:39</t>
-  </si>
-  <si>
-    <t>00:02:28</t>
-  </si>
-  <si>
-    <t>Apr 3 4:22PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Jimenez</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>03:55:13</t>
-  </si>
-  <si>
-    <t>00:03:49</t>
-  </si>
-  <si>
-    <t>00:04:16</t>
-  </si>
-  <si>
-    <t>00:01:43</t>
-  </si>
-  <si>
-    <t>00:00:26</t>
-  </si>
-  <si>
-    <t>Apr 3 5:50PM CST</t>
-  </si>
-  <si>
-    <t>Armando Muñoz</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>HINO 300</t>
-  </si>
-  <si>
-    <t>05:28:43</t>
-  </si>
-  <si>
-    <t>00:06:06</t>
-  </si>
-  <si>
-    <t>00:06:09</t>
-  </si>
-  <si>
-    <t>00:01:08</t>
-  </si>
-  <si>
-    <t>00:00:53</t>
-  </si>
-  <si>
-    <t>Apr 3 12:14PM CST</t>
-  </si>
-  <si>
-    <t>Fernando Garcia</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
-    <t>07:26:36</t>
-  </si>
-  <si>
-    <t>00:05:47</t>
-  </si>
-  <si>
-    <t>00:04:46</t>
-  </si>
-  <si>
-    <t>00:03:44</t>
-  </si>
-  <si>
-    <t>Apr 3 10:45AM CST</t>
-  </si>
-  <si>
-    <t>Daniel Mercado</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>03:00:39</t>
-  </si>
-  <si>
-    <t>00:02:37</t>
-  </si>
-  <si>
-    <t>00:01:49</t>
-  </si>
-  <si>
-    <t>Apr 3 2:30PM CST</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>03:59:47</t>
-  </si>
-  <si>
-    <t>00:02:45</t>
-  </si>
-  <si>
-    <t>00:02:48</t>
-  </si>
-  <si>
-    <t>00:01:44</t>
-  </si>
-  <si>
-    <t>Apr 3 12:43PM CST</t>
-  </si>
-  <si>
-    <t>David Serrano</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>03:09:10</t>
-  </si>
-  <si>
-    <t>00:03:05</t>
-  </si>
-  <si>
-    <t>00:00:17</t>
-  </si>
-  <si>
-    <t>Apr 3 1:17PM CST</t>
-  </si>
-  <si>
-    <t>Emmanuel Salcedo</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>02:44:25</t>
-  </si>
-  <si>
-    <t>00:00:44</t>
-  </si>
-  <si>
-    <t>00:00:28</t>
-  </si>
-  <si>
-    <t>Apr 3 3:33PM CST</t>
-  </si>
-  <si>
-    <t>Fernando Ornelas</t>
-  </si>
-  <si>
-    <t>138</t>
-  </si>
-  <si>
-    <t>02:02:44</t>
-  </si>
-  <si>
-    <t>00:01:01</t>
-  </si>
-  <si>
-    <t>00:00:46</t>
-  </si>
-  <si>
-    <t>Apr 3 2:51PM CST</t>
-  </si>
-  <si>
-    <t>Alberto Compras</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>NISSAN 1993</t>
-  </si>
-  <si>
-    <t>Sin ruta</t>
-  </si>
-  <si>
-    <t>Jorge Tornero</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>Martin Quezada</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>INTERNACIONAL</t>
-  </si>
-  <si>
-    <t>Miguel Zamora</t>
-  </si>
-  <si>
-    <t>139</t>
-  </si>
-  <si>
-    <t>Alexis Alvarado</t>
-  </si>
-  <si>
-    <t>145</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1226,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A36" sqref="A36"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1379,10 @@
         <v>35</v>
       </c>
       <c r="F2" s="1">
-        <v>77.900000000000006</v>
+        <v>53.3</v>
       </c>
       <c r="G2" s="1">
-        <v>9.7170000000000005</v>
+        <v>8.18</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -1376,10 +1394,10 @@
         <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -1394,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -1418,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA2" s="1">
         <v>0</v>
@@ -1444,40 +1462,40 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1">
-        <v>54.6</v>
+        <v>45.9</v>
       </c>
       <c r="G3" s="1">
-        <v>8.19</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -1492,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>45</v>
@@ -1516,10 +1534,10 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA3" s="1">
         <v>0</v>
@@ -1548,53 +1566,53 @@
         <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2">
         <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>54</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="1">
-        <v>43.6</v>
-      </c>
-      <c r="G4" s="1">
-        <v>7.7649999999999997</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>69.010000000000005</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="S4" s="1">
         <v>0</v>
       </c>
@@ -1614,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA4" s="1">
         <v>0</v>
@@ -1640,59 +1658,59 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1">
+        <v>42.1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7.01</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>56</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="1">
-        <v>29.2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4.875</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>43</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
@@ -1712,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA5" s="1">
         <v>0</v>
@@ -1738,13 +1756,13 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="2">
         <v>100</v>
@@ -1753,25 +1771,25 @@
         <v>58</v>
       </c>
       <c r="F6" s="1">
-        <v>28.5</v>
+        <v>31.5</v>
       </c>
       <c r="G6" s="1">
-        <v>5.1100000000000003</v>
+        <v>5.91</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -1786,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>59</v>
@@ -1810,10 +1828,10 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA6" s="1">
         <v>0</v>
@@ -1851,44 +1869,44 @@
         <v>63</v>
       </c>
       <c r="F7" s="1">
-        <v>21.5</v>
+        <v>25.4</v>
       </c>
       <c r="G7" s="1">
-        <v>3.8149999999999999</v>
+        <v>3.86</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>43</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>55</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="S7" s="1">
         <v>0</v>
       </c>
@@ -1908,10 +1926,10 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA7" s="1">
         <v>0</v>
@@ -1934,13 +1952,13 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
@@ -1949,25 +1967,25 @@
         <v>68</v>
       </c>
       <c r="F8" s="1">
-        <v>19.2</v>
+        <v>21.9</v>
       </c>
       <c r="G8" s="1">
-        <v>3.7559999999999998</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -1982,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -2006,10 +2024,10 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA8" s="1">
         <v>0</v>
@@ -2032,40 +2050,40 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2">
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F9" s="1">
-        <v>17.3</v>
+        <v>10.3</v>
       </c>
       <c r="G9" s="1">
-        <v>1.7390000000000001</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -2080,10 +2098,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -2104,10 +2122,10 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA9" s="1">
         <v>0</v>
@@ -2130,40 +2148,40 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2">
         <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="G10" s="1">
-        <v>1.2609999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -2178,10 +2196,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -2202,10 +2220,10 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA10" s="1">
         <v>0</v>
@@ -2228,40 +2246,40 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2">
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F11" s="1">
-        <v>4.2</v>
+        <v>0.2</v>
       </c>
       <c r="G11" s="1">
-        <v>1.899</v>
+        <v>1.5</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -2276,10 +2294,10 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -2300,10 +2318,10 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA11" s="1">
         <v>0</v>
@@ -2326,40 +2344,40 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D12" s="2">
         <v>100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" s="1">
-        <v>4.0999999999999996</v>
+        <v>0.1</v>
       </c>
       <c r="G12" s="1">
-        <v>1.5</v>
+        <v>0.11</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -2374,10 +2392,10 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -2398,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA12" s="1">
         <v>0</v>
@@ -2424,40 +2442,40 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D13" s="2">
         <v>100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F13" s="1">
-        <v>4</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>213</v>
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.31</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
@@ -2472,10 +2490,10 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1">
-        <v>49.59</v>
+        <v>9</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="S13" s="1">
         <v>0</v>
@@ -2496,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA13" s="1">
         <v>0</v>
@@ -2522,40 +2540,40 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D14" s="2">
+        <v>99</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="1">
+        <v>122.8</v>
+      </c>
+      <c r="G14" s="1">
+        <v>16.57</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="J14" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
@@ -2570,10 +2588,10 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1">
-        <v>18</v>
+        <v>90.01</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -2594,10 +2612,10 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA14" s="1">
         <v>0</v>
@@ -2620,40 +2638,40 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D15" s="2">
         <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F15" s="1">
-        <v>160.19999999999999</v>
+        <v>53.3</v>
       </c>
       <c r="G15" s="1">
-        <v>14.704000000000001</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
@@ -2668,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>96.01</v>
+        <v>70.010000000000005</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S15" s="1">
         <v>0</v>
@@ -2692,10 +2710,10 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA15" s="1">
         <v>0</v>
@@ -2718,40 +2736,40 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F16" s="1">
-        <v>53.6</v>
+        <v>153.69999999999999</v>
       </c>
       <c r="G16" s="1">
-        <v>7.5709999999999997</v>
+        <v>18.2</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
@@ -2766,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1">
-        <v>68.010000000000005</v>
+        <v>83.01</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
@@ -2790,10 +2808,10 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA16" s="1">
         <v>0</v>
@@ -2816,40 +2834,40 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D17" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F17" s="1">
-        <v>46.5</v>
+        <v>67.2</v>
       </c>
       <c r="G17" s="1">
-        <v>7.9820000000000011</v>
+        <v>9.42</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
@@ -2864,10 +2882,10 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>63</v>
+        <v>72.010000000000005</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="S17" s="1">
         <v>0</v>
@@ -2888,10 +2906,10 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA17" s="1">
         <v>0</v>
@@ -2914,40 +2932,40 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="D18" s="2">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F18" s="1">
-        <v>34.9</v>
+        <v>63.3</v>
       </c>
       <c r="G18" s="1">
-        <v>5.6539999999999999</v>
+        <v>8.91</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
@@ -2962,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1">
-        <v>68.010000000000005</v>
+        <v>84.01</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="S18" s="1">
         <v>0</v>
@@ -2986,10 +3004,10 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA18" s="1">
         <v>0</v>
@@ -3012,40 +3030,40 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="D19" s="2">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F19" s="1">
-        <v>65.3</v>
+        <v>45.3</v>
       </c>
       <c r="G19" s="1">
-        <v>10.183999999999999</v>
+        <v>7.63</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M19" s="1">
         <v>0</v>
@@ -3060,10 +3078,10 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1">
-        <v>73.010000000000005</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -3084,10 +3102,10 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA19" s="1">
         <v>0</v>
@@ -3110,40 +3128,40 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F20" s="1">
-        <v>68.900000000000006</v>
+        <v>61.1</v>
       </c>
       <c r="G20" s="1">
-        <v>10.656000000000001</v>
+        <v>12.71</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M20" s="1">
         <v>0</v>
@@ -3158,10 +3176,10 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1">
-        <v>81.010000000000005</v>
+        <v>79.010000000000005</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="S20" s="1">
         <v>0</v>
@@ -3182,10 +3200,10 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA20" s="1">
         <v>0</v>
@@ -3208,40 +3226,40 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D21" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F21" s="1">
-        <v>58.7</v>
-      </c>
-      <c r="G21" s="1">
-        <v>15.945</v>
+        <v>103.4</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M21" s="1">
         <v>0</v>
@@ -3256,10 +3274,10 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1">
-        <v>82.01</v>
+        <v>81.459999999999994</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -3280,10 +3298,10 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA21" s="1">
         <v>0</v>
@@ -3306,40 +3324,40 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="D22" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F22" s="1">
-        <v>56.2</v>
+        <v>136</v>
       </c>
       <c r="G22" s="1">
-        <v>9.6669999999999998</v>
+        <v>15.36</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
@@ -3354,10 +3372,10 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1">
-        <v>85.01</v>
+        <v>89.01</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="S22" s="1">
         <v>0</v>
@@ -3378,10 +3396,10 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA22" s="1">
         <v>0</v>
@@ -3404,46 +3422,46 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="D23" s="3">
         <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F23" s="1">
-        <v>180.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="G23" s="1">
-        <v>22.108000000000001</v>
+        <v>3.98</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="M23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1">
         <v>0</v>
@@ -3452,10 +3470,10 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>83.01</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="S23" s="1">
         <v>0</v>
@@ -3476,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA23" s="1">
         <v>0</v>
@@ -3502,40 +3520,40 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D24" s="3">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F24" s="1">
-        <v>134.6</v>
+        <v>58.8</v>
       </c>
       <c r="G24" s="1">
-        <v>19.908000000000001</v>
+        <v>5.58</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
@@ -3550,10 +3568,10 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>95.01</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="S24" s="1">
         <v>0</v>
@@ -3574,10 +3592,10 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA24" s="1">
         <v>0</v>
@@ -3600,46 +3618,46 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="3">
+        <v>85</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="1">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D25" s="3">
-        <v>72</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" s="1">
-        <v>360.2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>88.819000000000003</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -3648,10 +3666,10 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1">
-        <v>95.01</v>
+        <v>96.02</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="S25" s="1">
         <v>0</v>
@@ -3672,10 +3690,10 @@
         <v>0</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA25" s="1">
         <v>0</v>
@@ -3698,40 +3716,40 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D26" s="3">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F26" s="1">
-        <v>114.6</v>
+        <v>320.89999999999998</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>37</v>
+        <v>183</v>
       </c>
       <c r="M26" s="1">
         <v>0</v>
@@ -3746,10 +3764,10 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1">
-        <v>98.57</v>
+        <v>104.28</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="S26" s="1">
         <v>0</v>
@@ -3770,10 +3788,10 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA26" s="1">
         <v>0</v>
@@ -3796,40 +3814,40 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="D27" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F27" s="1">
-        <v>100</v>
+        <v>442.7</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="M27" s="1">
         <v>0</v>
@@ -3838,16 +3856,16 @@
         <v>0</v>
       </c>
       <c r="O27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="1">
         <v>0</v>
       </c>
       <c r="Q27" s="1">
-        <v>94.73</v>
+        <v>96.97</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
@@ -3868,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA27" s="1">
         <v>0</v>
@@ -3894,58 +3912,58 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D28" s="4">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F28" s="1">
-        <v>252.3</v>
+        <v>376.9</v>
       </c>
       <c r="G28" s="1">
-        <v>32.729999999999997</v>
+        <v>91.12</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
       </c>
       <c r="N28" s="1">
+        <v>4</v>
+      </c>
+      <c r="O28" s="1">
         <v>1</v>
       </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
       <c r="P28" s="1">
         <v>0</v>
       </c>
       <c r="Q28" s="1">
-        <v>90.01</v>
+        <v>97.01</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -3966,10 +3984,10 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA28" s="1">
         <v>0</v>
@@ -3992,40 +4010,40 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>201</v>
+        <v>104</v>
       </c>
       <c r="D29" s="4">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F29" s="1">
-        <v>356</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>213</v>
+        <v>116.2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>17.32</v>
       </c>
       <c r="H29" s="1">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>203</v>
+        <v>128</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="M29" s="1">
         <v>0</v>
@@ -4034,16 +4052,16 @@
         <v>0</v>
       </c>
       <c r="O29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="1">
-        <v>102.81</v>
+        <v>84.01</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S29" s="1">
         <v>0</v>
@@ -4064,10 +4082,10 @@
         <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA29" s="1">
         <v>0</v>
@@ -4090,46 +4108,46 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F30" s="1">
-        <v>58.3</v>
+        <v>219.5</v>
       </c>
       <c r="G30" s="1">
-        <v>8.1549999999999994</v>
+        <v>31.18</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>36</v>
+        <v>215</v>
       </c>
       <c r="M30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="1">
         <v>0</v>
@@ -4138,10 +4156,10 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1">
-        <v>79.010000000000005</v>
+        <v>134.01</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="S30" s="1">
         <v>0</v>
@@ -4162,10 +4180,10 @@
         <v>0</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA30" s="1">
         <v>0</v>
@@ -4188,40 +4206,40 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="D31" s="4">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F31" s="1">
-        <v>82.3</v>
+        <v>103.9</v>
       </c>
       <c r="G31" s="1">
-        <v>8.2669999999999995</v>
+        <v>14.1</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
@@ -4236,10 +4254,10 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1">
-        <v>94.01</v>
+        <v>80.010000000000005</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="S31" s="1">
         <v>0</v>
@@ -4260,10 +4278,10 @@
         <v>0</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA31" s="1">
         <v>0</v>
@@ -4275,7 +4293,7 @@
         <v>0</v>
       </c>
       <c r="AD31" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE31" s="1">
         <v>0</v>
@@ -4286,40 +4304,40 @@
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F32" s="1">
-        <v>64.599999999999994</v>
+        <v>58</v>
       </c>
       <c r="G32" s="1">
-        <v>5.7770000000000001</v>
+        <v>9.43</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>223</v>
+        <v>69</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="M32" s="1">
         <v>0</v>
@@ -4334,34 +4352,34 @@
         <v>0</v>
       </c>
       <c r="Q32" s="1">
-        <v>86.01</v>
+        <v>65.010000000000005</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="S32" s="1">
         <v>0</v>
       </c>
       <c r="T32" s="1">
+        <v>0</v>
+      </c>
+      <c r="U32" s="1">
+        <v>0</v>
+      </c>
+      <c r="V32" s="1">
+        <v>0</v>
+      </c>
+      <c r="W32" s="1">
+        <v>0</v>
+      </c>
+      <c r="X32" s="1">
         <v>1</v>
       </c>
-      <c r="U32" s="1">
-        <v>0</v>
-      </c>
-      <c r="V32" s="1">
-        <v>0</v>
-      </c>
-      <c r="W32" s="1">
-        <v>0</v>
-      </c>
-      <c r="X32" s="1">
-        <v>0</v>
-      </c>
       <c r="Y32" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA32" s="1">
         <v>0</v>
@@ -4384,40 +4402,40 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="D33" s="4">
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F33" s="1">
-        <v>50.3</v>
+        <v>44.8</v>
       </c>
       <c r="G33" s="1">
-        <v>9.532</v>
+        <v>8.43</v>
       </c>
       <c r="H33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>229</v>
+        <v>107</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>37</v>
+        <v>233</v>
       </c>
       <c r="M33" s="1">
         <v>0</v>
@@ -4432,10 +4450,10 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1">
-        <v>79.010000000000005</v>
+        <v>82.01</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="S33" s="1">
         <v>0</v>
@@ -4456,10 +4474,10 @@
         <v>0</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA33" s="1">
         <v>0</v>
@@ -4471,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="AD33" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE33" s="1">
         <v>0</v>
@@ -4482,40 +4500,40 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F34" s="1">
-        <v>34.4</v>
+        <v>41.6</v>
       </c>
       <c r="G34" s="1">
-        <v>5.8949999999999996</v>
+        <v>6.23</v>
       </c>
       <c r="H34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="M34" s="1">
         <v>0</v>
@@ -4530,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1">
-        <v>71.010000000000005</v>
+        <v>75.010000000000005</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="S34" s="1">
         <v>0</v>
@@ -4545,7 +4563,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W34" s="1">
         <v>0</v>
@@ -4554,10 +4572,10 @@
         <v>0</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA34" s="1">
         <v>0</v>
@@ -4569,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="AD34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE34" s="1">
         <v>0</v>
@@ -4580,492 +4598,492 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="P35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="R35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="S35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="T35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="U35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="V35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="W35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="X35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AC35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AD35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AE35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AF35" s="6" t="s">
-        <v>241</v>
+        <v>104</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3.77</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>94.01</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>1</v>
+      </c>
+      <c r="U35" s="1">
+        <v>0</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0</v>
+      </c>
+      <c r="X35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>192</v>
+        <v>248</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="U36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="X36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Y36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Z36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AA36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AB36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AC36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AD36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AE36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AF36" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="U37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="X37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Y37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Z37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AA37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AB37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AC37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AD37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AE37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AF37" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Q38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="R38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="U38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="V38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="W38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="X38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Z38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AA38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AB38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AC38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AD38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AE38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AF38" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="U39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="V39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Y39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="Z39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AA39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AB39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AC39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AD39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AE39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="AF39" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>